<commit_message>
final estimate of subash for pashu anudaan
</commit_message>
<xml_diff>
--- a/ofc/पशु शाखा इस्तिमेट/kamal.xlsx
+++ b/ofc/पशु शाखा इस्तिमेट/kamal.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\081-082\ofc\ofc\पशु शाखा इस्तिमेट\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\पशु शाखा इस्तिमेट\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="as per mistry" sheetId="19" r:id="rId1"/>
@@ -43,13 +43,13 @@
     <definedName name="description_784">[3]Abstract!$B$300</definedName>
     <definedName name="excavator">[2]Equipment_Rate!$J$19</definedName>
     <definedName name="generator">[2]Equipment_Rate!$J$20</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'as per mistry'!$A$1:$K$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'as per mistry'!$A$1:$K$46</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'as per mistry'!$1:$8</definedName>
     <definedName name="skilled">[2]District_Rate!$D$148</definedName>
     <definedName name="skilled_blacksmith">[2]District_Rate!$D$149</definedName>
     <definedName name="unskilled">[2]District_Rate!$D$156</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>no.</t>
-  </si>
-  <si>
-    <t>dfn;fdfg pknAw u/L )=%) dL=dL= afSnf] ;L=hL=cfO{= zL6 -h:tf kftfsf]_ 5fgf 5fpg] sfd k'/f .</t>
   </si>
   <si>
     <t>F1</t>
@@ -330,19 +327,22 @@
     <t xml:space="preserve">Date: 2082/02/05  </t>
   </si>
   <si>
-    <t>-MS square pipe of 1.5"*1.5" of 1.2mm thickness</t>
-  </si>
-  <si>
     <t>husf] vf8ndf 9'+uf eg]{ / n]en ug]{ sfddf</t>
+  </si>
+  <si>
+    <t>dfn;fdfg pknAw u/L )=@$ dL=dL= afSnf] ;L=hL=cfO{= zL6 -h:tf kftfsf]_ 5fgf 5fpg] sfd k'/f .</t>
+  </si>
+  <si>
+    <t>-MS square pipe of 1.5"*1.5" of 1.6mm thickness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -623,9 +623,9 @@
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -636,7 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,7 +644,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -661,7 +661,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -670,7 +670,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -682,7 +682,7 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -726,7 +726,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -821,10 +821,26 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -836,22 +852,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1666,139 +1666,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE48"/>
+  <dimension ref="A1:AE46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A32" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46:D46"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="22.5">
-      <c r="A2" s="78" t="s">
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="22.8">
+      <c r="A2" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-    </row>
-    <row r="5" spans="1:13" ht="18.75">
-      <c r="A5" s="80" t="s">
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+    </row>
+    <row r="5" spans="1:13" ht="17.399999999999999">
+      <c r="A5" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-    </row>
-    <row r="6" spans="1:13" ht="18.75">
-      <c r="A6" s="75" t="s">
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+    </row>
+    <row r="6" spans="1:13" ht="18">
+      <c r="A6" s="82" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.6">
+      <c r="A7" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="76" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="76"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75">
-      <c r="A7" s="83" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="76"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1">
       <c r="A8" s="3" t="s">
@@ -1835,7 +1835,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" ht="45">
+    <row r="9" spans="1:13" s="1" customFormat="1" ht="41.4">
       <c r="A9" s="21">
         <v>1</v>
       </c>
@@ -1860,10 +1860,10 @@
       <c r="J9" s="27"/>
       <c r="K9" s="24"/>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="27.6">
       <c r="A10" s="38"/>
       <c r="B10" s="39" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C10" s="40">
         <v>3</v>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="K14" s="24"/>
     </row>
-    <row r="15" spans="1:13" s="1" customFormat="1">
+    <row r="15" spans="1:13" s="1" customFormat="1" ht="15">
       <c r="A15" s="21"/>
       <c r="B15" s="37"/>
       <c r="C15" s="22"/>
@@ -2004,7 +2004,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="10"/>
@@ -2059,12 +2059,12 @@
         <v>31</v>
       </c>
       <c r="I18" s="26">
-        <f>7796.04/10</f>
-        <v>779.60400000000004</v>
+        <f>Sheet1!H10/10</f>
+        <v>249.75</v>
       </c>
       <c r="J18" s="27">
         <f>G18*I18</f>
-        <v>6286.1005441636062</v>
+        <v>2013.7834219743108</v>
       </c>
       <c r="K18" s="24"/>
     </row>
@@ -2119,25 +2119,24 @@
     <row r="22" spans="1:15" s="1" customFormat="1">
       <c r="A22" s="21"/>
       <c r="B22" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="22">
         <v>1</v>
       </c>
       <c r="D22" s="23">
-        <f>14.5/3.281</f>
-        <v>4.4193843340444987</v>
+        <v>4.5</v>
       </c>
       <c r="E22" s="24">
-        <f>10.25/3.281</f>
-        <v>3.1240475464797317</v>
+        <f>10/3.281</f>
+        <v>3.047851264858275</v>
       </c>
       <c r="F22" s="24">
         <v>0.15</v>
       </c>
       <c r="G22" s="36">
-        <f t="shared" ref="G22:G23" si="2">PRODUCT(C22:F22)</f>
-        <v>2.0709550178584015</v>
+        <f t="shared" ref="G22" si="2">PRODUCT(C22:F22)</f>
+        <v>2.0572996037793354</v>
       </c>
       <c r="H22" s="25"/>
       <c r="I22" s="26"/>
@@ -2146,57 +2145,49 @@
     </row>
     <row r="23" spans="1:15" s="1" customFormat="1">
       <c r="A23" s="21"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="22">
-        <v>1</v>
-      </c>
-      <c r="D23" s="23">
-        <v>4.5</v>
-      </c>
-      <c r="E23" s="24">
-        <f>10/3.281</f>
-        <v>3.047851264858275</v>
-      </c>
-      <c r="F23" s="24">
-        <v>0.15</v>
-      </c>
-      <c r="G23" s="36">
-        <f t="shared" si="2"/>
+      <c r="B23" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="27">
+        <f>SUM(G22:G22)</f>
         <v>2.0572996037793354</v>
       </c>
-      <c r="H23" s="25"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="27"/>
+      <c r="H23" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="26">
+        <v>663.31</v>
+      </c>
+      <c r="J23" s="27">
+        <f>G23*I23</f>
+        <v>1364.6274001828708</v>
+      </c>
       <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:15" s="1" customFormat="1">
       <c r="A24" s="21"/>
-      <c r="B24" s="39" t="s">
-        <v>25</v>
-      </c>
+      <c r="B24" s="39"/>
       <c r="C24" s="22"/>
       <c r="D24" s="23"/>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
-      <c r="G24" s="27">
-        <f>SUM(G22:G23)</f>
-        <v>4.1282546216377369</v>
-      </c>
-      <c r="H24" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="I24" s="26">
-        <v>663.31</v>
-      </c>
-      <c r="J24" s="27">
-        <f>G24*I24</f>
-        <v>2738.3125730785268</v>
-      </c>
+      <c r="G24" s="27"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="27"/>
       <c r="K24" s="24"/>
     </row>
-    <row r="25" spans="1:15" s="1" customFormat="1">
-      <c r="A25" s="21"/>
-      <c r="B25" s="39"/>
+    <row r="25" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A25" s="21">
+        <v>4</v>
+      </c>
+      <c r="B25" s="74" t="s">
+        <v>70</v>
+      </c>
       <c r="C25" s="22"/>
       <c r="D25" s="23"/>
       <c r="E25" s="24"/>
@@ -2207,18 +2198,31 @@
       <c r="J25" s="27"/>
       <c r="K25" s="24"/>
     </row>
-    <row r="26" spans="1:15" s="1" customFormat="1" ht="30">
-      <c r="A26" s="21">
-        <v>4</v>
-      </c>
-      <c r="B26" s="74" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="27"/>
+    <row r="26" spans="1:15" s="1" customFormat="1">
+      <c r="A26" s="21"/>
+      <c r="B26" s="39" t="str">
+        <f>B22</f>
+        <v>-for passage flooring</v>
+      </c>
+      <c r="C26" s="22">
+        <f>C22</f>
+        <v>1</v>
+      </c>
+      <c r="D26" s="23">
+        <f>D22</f>
+        <v>4.5</v>
+      </c>
+      <c r="E26" s="24">
+        <f>10/3.281</f>
+        <v>3.047851264858275</v>
+      </c>
+      <c r="F26" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="G26" s="36">
+        <f t="shared" ref="G26" si="3">PRODUCT(C26:F26)</f>
+        <v>2.0572996037793354</v>
+      </c>
       <c r="H26" s="25"/>
       <c r="I26" s="26"/>
       <c r="J26" s="27"/>
@@ -2226,90 +2230,78 @@
     </row>
     <row r="27" spans="1:15" s="1" customFormat="1">
       <c r="A27" s="21"/>
-      <c r="B27" s="39" t="str">
-        <f>B22</f>
-        <v>-for passage flooring</v>
-      </c>
-      <c r="C27" s="22">
-        <f>C22</f>
-        <v>1</v>
-      </c>
-      <c r="D27" s="23">
-        <f>D22</f>
-        <v>4.4193843340444987</v>
-      </c>
-      <c r="E27" s="24">
-        <f>E22</f>
-        <v>3.1240475464797317</v>
-      </c>
-      <c r="F27" s="24">
-        <v>0.15</v>
-      </c>
-      <c r="G27" s="36">
-        <f t="shared" ref="G27:G28" si="3">PRODUCT(C27:F27)</f>
-        <v>2.0709550178584015</v>
-      </c>
-      <c r="H27" s="25"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="27"/>
+      <c r="B27" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="27">
+        <f>SUM(G26:G26)</f>
+        <v>2.0572996037793354</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="26">
+        <v>4473.1499999999996</v>
+      </c>
+      <c r="J27" s="27">
+        <f>G27*I27</f>
+        <v>9202.6097226455331</v>
+      </c>
       <c r="K27" s="24"/>
     </row>
     <row r="28" spans="1:15" s="1" customFormat="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="22">
-        <f>C23</f>
-        <v>1</v>
-      </c>
-      <c r="D28" s="23">
-        <f>D23</f>
-        <v>4.5</v>
-      </c>
-      <c r="E28" s="24">
-        <f>E23</f>
-        <v>3.047851264858275</v>
-      </c>
-      <c r="F28" s="24">
-        <v>0.15</v>
-      </c>
-      <c r="G28" s="36">
-        <f t="shared" si="3"/>
-        <v>2.0572996037793354</v>
-      </c>
+      <c r="B28" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="27"/>
       <c r="H28" s="25"/>
       <c r="I28" s="26"/>
-      <c r="J28" s="27"/>
+      <c r="J28" s="27">
+        <f>0.13*G27*3093.15</f>
+        <v>827.25971502590676</v>
+      </c>
       <c r="K28" s="24"/>
+      <c r="M28" s="1">
+        <f>4434</f>
+        <v>4434</v>
+      </c>
+      <c r="N28" s="1" t="e">
+        <f>(PRODUCT(#REF!))*0.15+(PRODUCT(#REF!))*0.15+(PRODUCT(C26:E26))*0.15</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O28" s="1" t="e">
+        <f>N28*M28</f>
+        <v>#REF!</v>
+      </c>
     </row>
     <row r="29" spans="1:15" s="1" customFormat="1">
       <c r="A29" s="21"/>
-      <c r="B29" s="39" t="s">
-        <v>25</v>
-      </c>
+      <c r="B29" s="39"/>
       <c r="C29" s="22"/>
       <c r="D29" s="23"/>
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
-      <c r="G29" s="27">
-        <f>SUM(G27:G28)</f>
-        <v>4.1282546216377369</v>
-      </c>
-      <c r="H29" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" s="26">
-        <v>4473.1499999999996</v>
-      </c>
-      <c r="J29" s="27">
-        <f>G29*I29</f>
-        <v>18466.302160778843</v>
-      </c>
+      <c r="G29" s="27"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="27"/>
       <c r="K29" s="24"/>
     </row>
-    <row r="30" spans="1:15" s="1" customFormat="1">
-      <c r="A30" s="21"/>
-      <c r="B30" s="39" t="s">
-        <v>33</v>
+    <row r="30" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A30" s="21">
+        <v>5</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>37</v>
       </c>
       <c r="C30" s="22"/>
       <c r="D30" s="23"/>
@@ -2318,49 +2310,58 @@
       <c r="G30" s="27"/>
       <c r="H30" s="25"/>
       <c r="I30" s="26"/>
-      <c r="J30" s="27">
-        <f>0.13*G29*3093.15</f>
-        <v>1660.0104017794399</v>
-      </c>
+      <c r="J30" s="27"/>
       <c r="K30" s="24"/>
-      <c r="M30" s="1">
-        <f>4434</f>
-        <v>4434</v>
-      </c>
-      <c r="N30" s="1" t="e">
-        <f>(PRODUCT(#REF!))*0.15+(PRODUCT(C27:E27))*0.15+(PRODUCT(C28:E28))*0.15</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O30" s="1" t="e">
-        <f>N30*M30</f>
-        <v>#REF!</v>
-      </c>
     </row>
     <row r="31" spans="1:15" s="1" customFormat="1">
       <c r="A31" s="21"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="27"/>
+      <c r="B31" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="22">
+        <v>1</v>
+      </c>
+      <c r="D31" s="23">
+        <f>11/3.281</f>
+        <v>3.3526363913441024</v>
+      </c>
+      <c r="E31" s="24">
+        <f>8.25/3.281</f>
+        <v>2.5144772935080768</v>
+      </c>
+      <c r="F31" s="24">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G31" s="36">
+        <f>PRODUCT(C31:F31)</f>
+        <v>0.46365704436829819</v>
+      </c>
       <c r="H31" s="25"/>
       <c r="I31" s="26"/>
       <c r="J31" s="27"/>
       <c r="K31" s="24"/>
     </row>
-    <row r="32" spans="1:15" s="1" customFormat="1" ht="30">
-      <c r="A32" s="21">
-        <v>5</v>
-      </c>
-      <c r="B32" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="27"/>
+    <row r="32" spans="1:15" s="1" customFormat="1">
+      <c r="A32" s="21"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="22">
+        <v>1</v>
+      </c>
+      <c r="D32" s="23">
+        <f>14.5/3.281</f>
+        <v>4.4193843340444987</v>
+      </c>
+      <c r="E32" s="24">
+        <f>10.25/3.281</f>
+        <v>3.1240475464797317</v>
+      </c>
+      <c r="F32" s="24">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G32" s="36">
+        <f t="shared" ref="G32:G33" si="4">PRODUCT(C32:F32)</f>
+        <v>1.0354775089292008</v>
+      </c>
       <c r="H32" s="25"/>
       <c r="I32" s="26"/>
       <c r="J32" s="27"/>
@@ -2368,26 +2369,25 @@
     </row>
     <row r="33" spans="1:31" s="1" customFormat="1">
       <c r="A33" s="21"/>
-      <c r="B33" s="39" t="s">
-        <v>35</v>
-      </c>
+      <c r="B33" s="39"/>
       <c r="C33" s="22">
+        <f t="shared" ref="C33:E33" si="5">C26</f>
         <v>1</v>
       </c>
       <c r="D33" s="23">
-        <f>11/3.281</f>
-        <v>3.3526363913441024</v>
+        <f t="shared" si="5"/>
+        <v>4.5</v>
       </c>
       <c r="E33" s="24">
-        <f>8.25/3.281</f>
-        <v>2.5144772935080768</v>
+        <f t="shared" si="5"/>
+        <v>3.047851264858275</v>
       </c>
       <c r="F33" s="24">
-        <v>0.05</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="G33" s="36">
-        <f>PRODUCT(C33:F33)</f>
-        <v>0.42150640397118022</v>
+        <f t="shared" si="4"/>
+        <v>1.0286498018896677</v>
       </c>
       <c r="H33" s="25"/>
       <c r="I33" s="26"/>
@@ -2396,98 +2396,86 @@
     </row>
     <row r="34" spans="1:31" s="1" customFormat="1">
       <c r="A34" s="21"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="22">
-        <f t="shared" ref="C34:E34" si="4">C27</f>
-        <v>1</v>
-      </c>
-      <c r="D34" s="23">
-        <f t="shared" si="4"/>
-        <v>4.4193843340444987</v>
-      </c>
-      <c r="E34" s="24">
-        <f t="shared" si="4"/>
-        <v>3.1240475464797317</v>
-      </c>
-      <c r="F34" s="24">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="G34" s="36">
-        <f t="shared" ref="G34:G35" si="5">PRODUCT(C34:F34)</f>
-        <v>1.0354775089292008</v>
-      </c>
-      <c r="H34" s="25"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="27"/>
+      <c r="B34" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="27">
+        <f>SUM(G31:G33)</f>
+        <v>2.5277843551871664</v>
+      </c>
+      <c r="H34" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="I34" s="26">
+        <v>12983.1</v>
+      </c>
+      <c r="J34" s="27">
+        <f>G34*I34</f>
+        <v>32818.477061830497</v>
+      </c>
       <c r="K34" s="24"/>
     </row>
     <row r="35" spans="1:31" s="1" customFormat="1">
       <c r="A35" s="21"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="22">
-        <f t="shared" ref="C35:E35" si="6">C28</f>
-        <v>1</v>
-      </c>
-      <c r="D35" s="23">
-        <f t="shared" si="6"/>
-        <v>4.5</v>
-      </c>
-      <c r="E35" s="24">
-        <f t="shared" si="6"/>
-        <v>3.047851264858275</v>
-      </c>
-      <c r="F35" s="24">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="G35" s="36">
-        <f t="shared" si="5"/>
-        <v>1.0286498018896677</v>
-      </c>
+      <c r="B35" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="27"/>
       <c r="H35" s="25"/>
       <c r="I35" s="26"/>
-      <c r="J35" s="27"/>
+      <c r="J35" s="27">
+        <f>0.13*G34*8078.11</f>
+        <v>2654.5636100725301</v>
+      </c>
       <c r="K35" s="24"/>
     </row>
     <row r="36" spans="1:31" s="1" customFormat="1">
       <c r="A36" s="21"/>
-      <c r="B36" s="39" t="s">
-        <v>25</v>
-      </c>
+      <c r="B36" s="39"/>
       <c r="C36" s="22"/>
       <c r="D36" s="23"/>
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
-      <c r="G36" s="27">
-        <f>SUM(G33:G35)</f>
-        <v>2.4856337147900485</v>
-      </c>
-      <c r="H36" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="I36" s="26">
-        <v>12983.1</v>
-      </c>
-      <c r="J36" s="27">
-        <f>G36*I36</f>
-        <v>32271.231082490678</v>
-      </c>
+      <c r="G36" s="27"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="27"/>
       <c r="K36" s="24"/>
     </row>
     <row r="37" spans="1:31" s="1" customFormat="1">
-      <c r="A37" s="21"/>
-      <c r="B37" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="22"/>
+      <c r="A37" s="21">
+        <v>6</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="22">
+        <v>1</v>
+      </c>
       <c r="D37" s="23"/>
       <c r="E37" s="24"/>
       <c r="F37" s="24"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="26"/>
+      <c r="G37" s="36">
+        <f>PRODUCT(C37:F37)</f>
+        <v>1</v>
+      </c>
+      <c r="H37" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="I37" s="26">
+        <v>500</v>
+      </c>
       <c r="J37" s="27">
-        <f>0.13*G36*8078.11</f>
-        <v>2610.2989338117427</v>
+        <f>G37*I37</f>
+        <v>500</v>
       </c>
       <c r="K37" s="24"/>
     </row>
@@ -2504,74 +2492,99 @@
       <c r="J38" s="27"/>
       <c r="K38" s="24"/>
     </row>
-    <row r="39" spans="1:31" s="1" customFormat="1">
-      <c r="A39" s="21">
-        <v>6</v>
-      </c>
-      <c r="B39" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="22">
-        <v>1</v>
-      </c>
-      <c r="D39" s="23"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="36">
-        <f>PRODUCT(C39:F39)</f>
-        <v>1</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="I39" s="26">
-        <v>500</v>
-      </c>
-      <c r="J39" s="27">
-        <f>G39*I39</f>
-        <v>500</v>
-      </c>
-      <c r="K39" s="24"/>
-    </row>
-    <row r="40" spans="1:31" s="1" customFormat="1">
-      <c r="A40" s="21"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="24"/>
-    </row>
-    <row r="41" spans="1:31">
-      <c r="A41" s="9"/>
-      <c r="B41" s="20" t="s">
+    <row r="39" spans="1:31">
+      <c r="A39" s="9"/>
+      <c r="B39" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7">
-        <f>SUM(J10:J40)</f>
-        <v>68685.877896601742</v>
-      </c>
-      <c r="K41" s="4"/>
-      <c r="M41" s="29"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7">
+        <f>SUM(J10:J38)</f>
+        <v>53534.943132230554</v>
+      </c>
+      <c r="K39" s="4"/>
+      <c r="M39" s="29"/>
+      <c r="P39" s="32"/>
+      <c r="Q39" s="32"/>
+    </row>
+    <row r="40" spans="1:31">
+      <c r="M40" s="29"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="31"/>
+      <c r="R40" s="30"/>
+      <c r="S40" s="30"/>
+      <c r="T40" s="30"/>
+      <c r="U40" s="29"/>
+      <c r="V40" s="29"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="29"/>
+    </row>
+    <row r="41" spans="1:31" s="1" customFormat="1">
+      <c r="B41" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="75">
+        <f>J39</f>
+        <v>53534.943132230554</v>
+      </c>
+      <c r="D41" s="76"/>
+      <c r="E41" s="10">
+        <v>100</v>
+      </c>
+      <c r="F41" s="12"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="16"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="S41" s="30"/>
+      <c r="T41" s="30"/>
+      <c r="U41" s="12"/>
+      <c r="V41" s="12"/>
+      <c r="W41" s="12"/>
+      <c r="X41" s="12"/>
+      <c r="Y41" s="12"/>
+      <c r="Z41" s="12"/>
+      <c r="AA41" s="12"/>
+      <c r="AB41" s="12"/>
+      <c r="AC41" s="12"/>
+      <c r="AD41" s="12"/>
+      <c r="AE41" s="12"/>
     </row>
     <row r="42" spans="1:31">
+      <c r="B42" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="79">
+        <v>60000</v>
+      </c>
+      <c r="D42" s="80"/>
+      <c r="E42" s="10"/>
       <c r="M42" s="29"/>
       <c r="N42" s="30"/>
       <c r="O42" s="30"/>
-      <c r="P42" s="31"/>
+      <c r="P42" s="30"/>
+      <c r="Q42" s="30"/>
       <c r="R42" s="30"/>
       <c r="S42" s="30"/>
       <c r="T42" s="30"/>
@@ -2587,61 +2600,59 @@
       <c r="AD42" s="29"/>
       <c r="AE42" s="29"/>
     </row>
-    <row r="43" spans="1:31" s="1" customFormat="1">
+    <row r="43" spans="1:31">
       <c r="B43" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C43" s="81">
-        <f>J41</f>
-        <v>68685.877896601742</v>
-      </c>
-      <c r="D43" s="82"/>
+        <v>18</v>
+      </c>
+      <c r="C43" s="79">
+        <v>30000</v>
+      </c>
+      <c r="D43" s="80"/>
       <c r="E43" s="10">
-        <v>100</v>
-      </c>
-      <c r="F43" s="12"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="16"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="30"/>
-      <c r="O43" s="30"/>
-      <c r="P43" s="30"/>
-      <c r="Q43" s="30"/>
-      <c r="R43" s="30"/>
-      <c r="S43" s="30"/>
-      <c r="T43" s="30"/>
-      <c r="U43" s="12"/>
-      <c r="V43" s="12"/>
-      <c r="W43" s="12"/>
-      <c r="X43" s="12"/>
-      <c r="Y43" s="12"/>
-      <c r="Z43" s="12"/>
-      <c r="AA43" s="12"/>
-      <c r="AB43" s="12"/>
-      <c r="AC43" s="12"/>
-      <c r="AD43" s="12"/>
-      <c r="AE43" s="12"/>
+        <f>C43/C41*100</f>
+        <v>56.038165438787189</v>
+      </c>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="29"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="29"/>
+      <c r="AB43" s="29"/>
+      <c r="AC43" s="29"/>
+      <c r="AD43" s="29"/>
+      <c r="AE43" s="29"/>
     </row>
     <row r="44" spans="1:31">
       <c r="B44" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" s="84">
-        <v>60000</v>
-      </c>
-      <c r="D44" s="85"/>
-      <c r="E44" s="10"/>
+        <v>19</v>
+      </c>
+      <c r="C44" s="81">
+        <f>C41-C43</f>
+        <v>23534.943132230554</v>
+      </c>
+      <c r="D44" s="81"/>
+      <c r="E44" s="10">
+        <f>100-E43</f>
+        <v>43.961834561212811</v>
+      </c>
       <c r="M44" s="29"/>
-      <c r="N44" s="30"/>
-      <c r="O44" s="30"/>
-      <c r="P44" s="30"/>
-      <c r="Q44" s="30"/>
-      <c r="R44" s="30"/>
-      <c r="S44" s="30"/>
-      <c r="T44" s="30"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
       <c r="U44" s="29"/>
       <c r="V44" s="29"/>
       <c r="W44" s="29"/>
@@ -2656,15 +2667,15 @@
     </row>
     <row r="45" spans="1:31">
       <c r="B45" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C45" s="84">
-        <v>30000</v>
-      </c>
-      <c r="D45" s="85"/>
+        <v>20</v>
+      </c>
+      <c r="C45" s="75">
+        <f>C42*0.03</f>
+        <v>1800</v>
+      </c>
+      <c r="D45" s="76"/>
       <c r="E45" s="10">
-        <f>C45/C43*100</f>
-        <v>43.677100619084122</v>
+        <v>3</v>
       </c>
       <c r="M45" s="29"/>
       <c r="N45" s="29"/>
@@ -2688,16 +2699,15 @@
     </row>
     <row r="46" spans="1:31">
       <c r="B46" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" s="86">
-        <f>C43-C45</f>
-        <v>38685.877896601742</v>
-      </c>
-      <c r="D46" s="86"/>
+        <v>21</v>
+      </c>
+      <c r="C46" s="75">
+        <f>C42*0.02</f>
+        <v>1200</v>
+      </c>
+      <c r="D46" s="76"/>
       <c r="E46" s="10">
-        <f>100-E45</f>
-        <v>56.322899380915878</v>
+        <v>2</v>
       </c>
       <c r="M46" s="29"/>
       <c r="N46" s="29"/>
@@ -2719,80 +2729,8 @@
       <c r="AD46" s="29"/>
       <c r="AE46" s="29"/>
     </row>
-    <row r="47" spans="1:31">
-      <c r="B47" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="81">
-        <f>C44*0.03</f>
-        <v>1800</v>
-      </c>
-      <c r="D47" s="82"/>
-      <c r="E47" s="10">
-        <v>3</v>
-      </c>
-      <c r="M47" s="29"/>
-      <c r="N47" s="29"/>
-      <c r="O47" s="29"/>
-      <c r="P47" s="29"/>
-      <c r="Q47" s="29"/>
-      <c r="R47" s="29"/>
-      <c r="S47" s="29"/>
-      <c r="T47" s="29"/>
-      <c r="U47" s="29"/>
-      <c r="V47" s="29"/>
-      <c r="W47" s="29"/>
-      <c r="X47" s="29"/>
-      <c r="Y47" s="29"/>
-      <c r="Z47" s="29"/>
-      <c r="AA47" s="29"/>
-      <c r="AB47" s="29"/>
-      <c r="AC47" s="29"/>
-      <c r="AD47" s="29"/>
-      <c r="AE47" s="29"/>
-    </row>
-    <row r="48" spans="1:31">
-      <c r="B48" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="81">
-        <f>C44*0.02</f>
-        <v>1200</v>
-      </c>
-      <c r="D48" s="82"/>
-      <c r="E48" s="10">
-        <v>2</v>
-      </c>
-      <c r="M48" s="29"/>
-      <c r="N48" s="29"/>
-      <c r="O48" s="29"/>
-      <c r="P48" s="29"/>
-      <c r="Q48" s="29"/>
-      <c r="R48" s="29"/>
-      <c r="S48" s="29"/>
-      <c r="T48" s="29"/>
-      <c r="U48" s="29"/>
-      <c r="V48" s="29"/>
-      <c r="W48" s="29"/>
-      <c r="X48" s="29"/>
-      <c r="Y48" s="29"/>
-      <c r="Z48" s="29"/>
-      <c r="AA48" s="29"/>
-      <c r="AB48" s="29"/>
-      <c r="AC48" s="29"/>
-      <c r="AD48" s="29"/>
-      <c r="AE48" s="29"/>
-    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -2800,6 +2738,14 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2815,21 +2761,21 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="43" customFormat="1" ht="20.100000000000001" customHeight="1">
@@ -2838,7 +2784,7 @@
         <v>#REF!</v>
       </c>
       <c r="B1" s="87" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="C1" s="88"/>
       <c r="D1" s="88"/>
@@ -2849,10 +2795,10 @@
     </row>
     <row r="2" spans="1:8" s="43" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="89" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" s="89" t="s">
-        <v>41</v>
       </c>
       <c r="C2" s="90"/>
       <c r="D2" s="90"/>
@@ -2863,39 +2809,39 @@
     </row>
     <row r="3" spans="1:8" s="43" customFormat="1" ht="33" customHeight="1">
       <c r="B3" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="D3" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="E3" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="F3" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="G3" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="H3" s="45" t="s">
         <v>47</v>
-      </c>
-      <c r="H3" s="45" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="43" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="B4" s="91" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="46" t="s">
         <v>49</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>50</v>
       </c>
       <c r="D4" s="47">
         <v>1.1000000000000001</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="49">
         <v>1225</v>
@@ -2909,13 +2855,13 @@
     <row r="5" spans="1:8" s="43" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="B5" s="92"/>
       <c r="C5" s="51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="52">
         <v>1.25</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="53">
         <v>920</v>
@@ -2929,18 +2875,18 @@
         <v>2497.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="43" customFormat="1" ht="16.5">
+    <row r="6" spans="1:8" s="43" customFormat="1" ht="16.2">
       <c r="B6" s="93" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="56">
         <v>12</v>
       </c>
       <c r="E6" s="57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="58">
         <f>313.4529148</f>
@@ -2952,16 +2898,16 @@
       </c>
       <c r="H6" s="59"/>
     </row>
-    <row r="7" spans="1:8" s="43" customFormat="1" ht="16.5">
+    <row r="7" spans="1:8" s="43" customFormat="1" ht="16.2">
       <c r="B7" s="94"/>
       <c r="C7" s="57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="56">
         <v>30</v>
       </c>
       <c r="E7" s="57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="58">
         <v>34.130000000000003</v>
@@ -2975,13 +2921,13 @@
     <row r="8" spans="1:8" s="43" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="B8" s="94"/>
       <c r="C8" s="57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="56">
         <v>25</v>
       </c>
       <c r="E8" s="57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F8" s="58">
         <f>'[1]update Rate'!$N$131</f>
@@ -2996,13 +2942,13 @@
     <row r="9" spans="1:8" s="61" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="B9" s="95"/>
       <c r="C9" s="62" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" s="63">
         <v>55</v>
       </c>
       <c r="E9" s="62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" s="64">
         <f>'[1]update Rate'!$N$132</f>
@@ -3013,56 +2959,56 @@
         <v>165</v>
       </c>
       <c r="H9" s="65">
-        <f>SUM(G6+G7+G8+G9)</f>
-        <v>5298.54</v>
+        <f>0*SUM(G6+G7+G8+G9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="43" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="F10" s="43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" s="66"/>
       <c r="H10" s="53">
         <f>SUM(H5:H9)</f>
-        <v>7796.04</v>
+        <v>2497.5</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="43" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="B11" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="43" t="s">
         <v>60</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>61</v>
       </c>
       <c r="G11" s="66"/>
       <c r="H11" s="68">
         <f>FLOOR(H10*0.15,0.01)</f>
-        <v>1169.4000000000001</v>
+        <v>374.62</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="43" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="69"/>
       <c r="B12" s="70">
         <f>+H12</f>
-        <v>8965.44</v>
+        <v>2872.12</v>
       </c>
       <c r="C12" s="69" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="71">
         <f>INT(B12/B13*100)/100</f>
-        <v>896.54</v>
+        <v>287.20999999999998</v>
       </c>
       <c r="E12" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="43" t="s">
         <v>63</v>
-      </c>
-      <c r="F12" s="43" t="s">
-        <v>64</v>
       </c>
       <c r="G12" s="66"/>
       <c r="H12" s="71">
         <f>SUM(H10:H11)</f>
-        <v>8965.44</v>
+        <v>2872.12</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="43" customFormat="1" ht="20.100000000000001" customHeight="1">
@@ -3070,9 +3016,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="43" customFormat="1">
+    <row r="14" spans="1:8" s="43" customFormat="1" ht="15">
       <c r="A14" s="73" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
construction of new ghar kurthali complete
</commit_message>
<xml_diff>
--- a/ofc/पशु शाखा इस्तिमेट/kamal.xlsx
+++ b/ofc/पशु शाखा इस्तिमेट/kamal.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\पशु शाखा इस्तिमेट\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\081-082\ofc\ofc\पशु शाखा इस्तिमेट\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="as per mistry" sheetId="19" r:id="rId1"/>
@@ -43,13 +43,13 @@
     <definedName name="description_784">[3]Abstract!$B$300</definedName>
     <definedName name="excavator">[2]Equipment_Rate!$J$19</definedName>
     <definedName name="generator">[2]Equipment_Rate!$J$20</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'as per mistry'!$A$1:$K$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'as per mistry'!$A$1:$K$48</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'as per mistry'!$1:$8</definedName>
     <definedName name="skilled">[2]District_Rate!$D$148</definedName>
     <definedName name="skilled_blacksmith">[2]District_Rate!$D$149</definedName>
     <definedName name="unskilled">[2]District_Rate!$D$156</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -339,10 +339,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -623,9 +623,9 @@
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -636,7 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,7 +644,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -661,7 +661,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -670,7 +670,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -682,7 +682,7 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -726,7 +726,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -821,6 +821,22 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -828,9 +844,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -839,19 +852,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1312,33 +1312,33 @@
       <sheetName val="PPMO_BOQ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
         <row r="33">
           <cell r="B33" t="str">
             <v>Earthwork Excavation in Cutting., Roadway Excavation in all types of Soil by Manual Means ., Roadway Excavation in all types of soil as per drawing and technical specification, including removal of stumps and other deleterious matter, with all lifts and lead as per Drawing and instruction of the Engineer.</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1666,139 +1666,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE46"/>
+  <dimension ref="A1:AE48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="22.8">
-      <c r="A2" s="84" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="22.5">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-    </row>
-    <row r="5" spans="1:13" ht="17.399999999999999">
-      <c r="A5" s="86" t="s">
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+    </row>
+    <row r="5" spans="1:13" ht="18.75">
+      <c r="A5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="86"/>
-    </row>
-    <row r="6" spans="1:13" ht="18">
-      <c r="A6" s="82" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+    </row>
+    <row r="6" spans="1:13" ht="18.75">
+      <c r="A6" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="78" t="s">
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.6">
-      <c r="A7" s="77" t="s">
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75">
+      <c r="A7" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="78" t="s">
+      <c r="H7" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1">
       <c r="A8" s="3" t="s">
@@ -1835,7 +1835,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" ht="41.4">
+    <row r="9" spans="1:13" s="1" customFormat="1" ht="45">
       <c r="A9" s="21">
         <v>1</v>
       </c>
@@ -1860,7 +1860,7 @@
       <c r="J9" s="27"/>
       <c r="K9" s="24"/>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" ht="27.6">
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A10" s="38"/>
       <c r="B10" s="39" t="s">
         <v>72</v>
@@ -1944,167 +1944,188 @@
       <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1">
-      <c r="A13" s="21"/>
-      <c r="B13" s="39" t="s">
+      <c r="A13" s="38"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40">
+        <v>3</v>
+      </c>
+      <c r="D13" s="10">
+        <f>10/3.281</f>
+        <v>3.047851264858275</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1.83</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" ref="F13:F14" si="2">PRODUCT(C13:E13)</f>
+        <v>16.73270344407193</v>
+      </c>
+      <c r="G13" s="36">
+        <f t="shared" ref="G13:G14" si="3">F13</f>
+        <v>16.73270344407193</v>
+      </c>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="11"/>
+      <c r="M13" s="12"/>
+    </row>
+    <row r="14" spans="1:13" s="1" customFormat="1">
+      <c r="A14" s="38"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="40">
+        <v>3</v>
+      </c>
+      <c r="D14" s="10">
+        <f>7.5/3.281</f>
+        <v>2.2858884486437061</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1.83</v>
+      </c>
+      <c r="F14" s="10">
+        <f t="shared" si="2"/>
+        <v>12.549527583053948</v>
+      </c>
+      <c r="G14" s="36">
+        <f t="shared" si="3"/>
+        <v>12.549527583053948</v>
+      </c>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="11"/>
+      <c r="M14" s="12"/>
+    </row>
+    <row r="15" spans="1:13" s="1" customFormat="1">
+      <c r="A15" s="21"/>
+      <c r="B15" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="27">
-        <f>SUM(G10:G12)</f>
-        <v>18.546095306309052</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="26">
-        <v>181.17</v>
-      </c>
-      <c r="J13" s="27">
-        <f>G13*I13</f>
-        <v>3359.9960866440106</v>
-      </c>
-      <c r="K13" s="24"/>
-    </row>
-    <row r="14" spans="1:13" s="1" customFormat="1">
-      <c r="A14" s="21"/>
-      <c r="B14" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27">
-        <f>0.13*G13*(1871.42/18.94)</f>
-        <v>238.2248879702891</v>
-      </c>
-      <c r="K14" s="24"/>
-    </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" ht="15">
-      <c r="A15" s="21"/>
-      <c r="B15" s="37"/>
       <c r="C15" s="22"/>
       <c r="D15" s="23"/>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
+      <c r="G15" s="27">
+        <f>SUM(G10:G14)</f>
+        <v>47.82832633343493</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="26">
+        <v>181.17</v>
+      </c>
+      <c r="J15" s="27">
+        <f>G15*I15</f>
+        <v>8665.0578818284048</v>
+      </c>
       <c r="K15" s="24"/>
     </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" ht="30">
-      <c r="A16" s="38">
+    <row r="16" spans="1:13" s="1" customFormat="1">
+      <c r="A16" s="21"/>
+      <c r="B16" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27">
+        <f>0.13*G15*(1871.42/18.94)</f>
+        <v>614.35560932941837</v>
+      </c>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:15" s="1" customFormat="1">
+      <c r="A17" s="21"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="24"/>
+    </row>
+    <row r="18" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A18" s="38">
         <v>2</v>
       </c>
-      <c r="B16" s="74" t="s">
+      <c r="B18" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="11"/>
-      <c r="M16" s="12"/>
-    </row>
-    <row r="17" spans="1:15" s="1" customFormat="1">
-      <c r="A17" s="38"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="40">
+      <c r="C18" s="40"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="11"/>
+      <c r="M18" s="12"/>
+    </row>
+    <row r="19" spans="1:15" s="1" customFormat="1">
+      <c r="A19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="40">
         <v>5</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D19" s="10">
         <f>8/3.281</f>
         <v>2.4382810118866196</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E19" s="10">
         <f>2.17/3.281</f>
         <v>0.66138372447424565</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="36">
-        <f>PRODUCT(C17:F17)</f>
+      <c r="F19" s="10"/>
+      <c r="G19" s="36">
+        <f>PRODUCT(C19:F19)</f>
         <v>8.063196884782025</v>
       </c>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="11"/>
-      <c r="M17" s="12"/>
-    </row>
-    <row r="18" spans="1:15" s="1" customFormat="1">
-      <c r="A18" s="21"/>
-      <c r="B18" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="27">
-        <f>SUM(G17:G17)</f>
-        <v>8.063196884782025</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="26">
-        <f>Sheet1!H10/10</f>
-        <v>249.75</v>
-      </c>
-      <c r="J18" s="27">
-        <f>G18*I18</f>
-        <v>2013.7834219743108</v>
-      </c>
-      <c r="K18" s="24"/>
-    </row>
-    <row r="19" spans="1:15" s="1" customFormat="1">
-      <c r="A19" s="21"/>
-      <c r="B19" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="27">
-        <f>0.13*G18*5298.54/10</f>
-        <v>555.40122588460849</v>
-      </c>
-      <c r="K19" s="24"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="11"/>
+      <c r="M19" s="12"/>
     </row>
     <row r="20" spans="1:15" s="1" customFormat="1">
       <c r="A20" s="21"/>
-      <c r="B20" s="39"/>
+      <c r="B20" s="39" t="s">
+        <v>25</v>
+      </c>
       <c r="C20" s="22"/>
       <c r="D20" s="23"/>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="27"/>
+      <c r="G20" s="27">
+        <f>SUM(G19:G19)</f>
+        <v>8.063196884782025</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="26">
+        <f>Sheet1!H10/10</f>
+        <v>249.75</v>
+      </c>
+      <c r="J20" s="27">
+        <f>G20*I20</f>
+        <v>2013.7834219743108</v>
+      </c>
       <c r="K20" s="24"/>
     </row>
-    <row r="21" spans="1:15" s="1" customFormat="1" ht="30">
-      <c r="A21" s="21">
-        <v>3</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>34</v>
+    <row r="21" spans="1:15" s="1" customFormat="1">
+      <c r="A21" s="21"/>
+      <c r="B21" s="39" t="s">
+        <v>33</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
@@ -2113,195 +2134,183 @@
       <c r="G21" s="27"/>
       <c r="H21" s="25"/>
       <c r="I21" s="26"/>
-      <c r="J21" s="27"/>
+      <c r="J21" s="27">
+        <f>0*0.13*G20*5298.54/10</f>
+        <v>0</v>
+      </c>
       <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:15" s="1" customFormat="1">
       <c r="A22" s="21"/>
-      <c r="B22" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="22">
-        <v>1</v>
-      </c>
-      <c r="D22" s="23">
-        <v>4.5</v>
-      </c>
-      <c r="E22" s="24">
-        <f>10/3.281</f>
-        <v>3.047851264858275</v>
-      </c>
-      <c r="F22" s="24">
-        <v>0.15</v>
-      </c>
-      <c r="G22" s="36">
-        <f t="shared" ref="G22" si="2">PRODUCT(C22:F22)</f>
-        <v>2.0572996037793354</v>
-      </c>
+      <c r="B22" s="39"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="27"/>
       <c r="H22" s="25"/>
       <c r="I22" s="26"/>
       <c r="J22" s="27"/>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="1:15" s="1" customFormat="1">
-      <c r="A23" s="21"/>
-      <c r="B23" s="39" t="s">
-        <v>25</v>
+    <row r="23" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A23" s="21">
+        <v>3</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>34</v>
       </c>
       <c r="C23" s="22"/>
       <c r="D23" s="23"/>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
-      <c r="G23" s="27">
-        <f>SUM(G22:G22)</f>
-        <v>2.0572996037793354</v>
-      </c>
-      <c r="H23" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="I23" s="26">
-        <v>663.31</v>
-      </c>
-      <c r="J23" s="27">
-        <f>G23*I23</f>
-        <v>1364.6274001828708</v>
-      </c>
+      <c r="G23" s="27"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="27"/>
       <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:15" s="1" customFormat="1">
       <c r="A24" s="21"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="27"/>
+      <c r="B24" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="22">
+        <v>1</v>
+      </c>
+      <c r="D24" s="23">
+        <v>4.5</v>
+      </c>
+      <c r="E24" s="24">
+        <f>10/3.281</f>
+        <v>3.047851264858275</v>
+      </c>
+      <c r="F24" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="G24" s="36">
+        <f t="shared" ref="G24" si="4">PRODUCT(C24:F24)</f>
+        <v>2.0572996037793354</v>
+      </c>
       <c r="H24" s="25"/>
       <c r="I24" s="26"/>
       <c r="J24" s="27"/>
       <c r="K24" s="24"/>
     </row>
-    <row r="25" spans="1:15" s="1" customFormat="1" ht="30">
-      <c r="A25" s="21">
-        <v>4</v>
-      </c>
-      <c r="B25" s="74" t="s">
-        <v>70</v>
+    <row r="25" spans="1:15" s="1" customFormat="1">
+      <c r="A25" s="21"/>
+      <c r="B25" s="39" t="s">
+        <v>25</v>
       </c>
       <c r="C25" s="22"/>
       <c r="D25" s="23"/>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="27"/>
+      <c r="G25" s="27">
+        <f>SUM(G24:G24)</f>
+        <v>2.0572996037793354</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="I25" s="26">
+        <v>663.31</v>
+      </c>
+      <c r="J25" s="27">
+        <f>G25*I25</f>
+        <v>1364.6274001828708</v>
+      </c>
       <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:15" s="1" customFormat="1">
       <c r="A26" s="21"/>
-      <c r="B26" s="39" t="str">
-        <f>B22</f>
-        <v>-for passage flooring</v>
-      </c>
-      <c r="C26" s="22">
-        <f>C22</f>
-        <v>1</v>
-      </c>
-      <c r="D26" s="23">
-        <f>D22</f>
-        <v>4.5</v>
-      </c>
-      <c r="E26" s="24">
-        <f>10/3.281</f>
-        <v>3.047851264858275</v>
-      </c>
-      <c r="F26" s="24">
-        <v>0.15</v>
-      </c>
-      <c r="G26" s="36">
-        <f t="shared" ref="G26" si="3">PRODUCT(C26:F26)</f>
-        <v>2.0572996037793354</v>
-      </c>
+      <c r="B26" s="39"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="27"/>
       <c r="H26" s="25"/>
       <c r="I26" s="26"/>
       <c r="J26" s="27"/>
       <c r="K26" s="24"/>
     </row>
-    <row r="27" spans="1:15" s="1" customFormat="1">
-      <c r="A27" s="21"/>
-      <c r="B27" s="39" t="s">
-        <v>25</v>
+    <row r="27" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A27" s="21">
+        <v>4</v>
+      </c>
+      <c r="B27" s="74" t="s">
+        <v>70</v>
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="23"/>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
-      <c r="G27" s="27">
-        <f>SUM(G26:G26)</f>
-        <v>2.0572996037793354</v>
-      </c>
-      <c r="H27" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="I27" s="26">
-        <v>4473.1499999999996</v>
-      </c>
-      <c r="J27" s="27">
-        <f>G27*I27</f>
-        <v>9202.6097226455331</v>
-      </c>
+      <c r="G27" s="27"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="27"/>
       <c r="K27" s="24"/>
     </row>
     <row r="28" spans="1:15" s="1" customFormat="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="27"/>
+      <c r="B28" s="39" t="str">
+        <f>B24</f>
+        <v>-for passage flooring</v>
+      </c>
+      <c r="C28" s="22">
+        <f>C24</f>
+        <v>1</v>
+      </c>
+      <c r="D28" s="23">
+        <f>D24</f>
+        <v>4.5</v>
+      </c>
+      <c r="E28" s="24">
+        <f>10/3.281</f>
+        <v>3.047851264858275</v>
+      </c>
+      <c r="F28" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="G28" s="36">
+        <f t="shared" ref="G28" si="5">PRODUCT(C28:F28)</f>
+        <v>2.0572996037793354</v>
+      </c>
       <c r="H28" s="25"/>
       <c r="I28" s="26"/>
-      <c r="J28" s="27">
-        <f>0.13*G27*3093.15</f>
-        <v>827.25971502590676</v>
-      </c>
+      <c r="J28" s="27"/>
       <c r="K28" s="24"/>
-      <c r="M28" s="1">
-        <f>4434</f>
-        <v>4434</v>
-      </c>
-      <c r="N28" s="1" t="e">
-        <f>(PRODUCT(#REF!))*0.15+(PRODUCT(#REF!))*0.15+(PRODUCT(C26:E26))*0.15</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O28" s="1" t="e">
-        <f>N28*M28</f>
-        <v>#REF!</v>
-      </c>
     </row>
     <row r="29" spans="1:15" s="1" customFormat="1">
       <c r="A29" s="21"/>
-      <c r="B29" s="39"/>
+      <c r="B29" s="39" t="s">
+        <v>25</v>
+      </c>
       <c r="C29" s="22"/>
       <c r="D29" s="23"/>
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="27"/>
+      <c r="G29" s="27">
+        <f>SUM(G28:G28)</f>
+        <v>2.0572996037793354</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="26">
+        <v>4473.1499999999996</v>
+      </c>
+      <c r="J29" s="27">
+        <f>G29*I29</f>
+        <v>9202.6097226455331</v>
+      </c>
       <c r="K29" s="24"/>
     </row>
-    <row r="30" spans="1:15" s="1" customFormat="1" ht="30">
-      <c r="A30" s="21">
-        <v>5</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>37</v>
+    <row r="30" spans="1:15" s="1" customFormat="1">
+      <c r="A30" s="21"/>
+      <c r="B30" s="39" t="s">
+        <v>33</v>
       </c>
       <c r="C30" s="22"/>
       <c r="D30" s="23"/>
@@ -2310,58 +2319,49 @@
       <c r="G30" s="27"/>
       <c r="H30" s="25"/>
       <c r="I30" s="26"/>
-      <c r="J30" s="27"/>
+      <c r="J30" s="27">
+        <f>0.13*G29*3093.15</f>
+        <v>827.25971502590676</v>
+      </c>
       <c r="K30" s="24"/>
+      <c r="M30" s="1">
+        <f>4434</f>
+        <v>4434</v>
+      </c>
+      <c r="N30" s="1" t="e">
+        <f>(PRODUCT(#REF!))*0.15+(PRODUCT(#REF!))*0.15+(PRODUCT(C28:E28))*0.15</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O30" s="1" t="e">
+        <f>N30*M30</f>
+        <v>#REF!</v>
+      </c>
     </row>
     <row r="31" spans="1:15" s="1" customFormat="1">
       <c r="A31" s="21"/>
-      <c r="B31" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="22">
-        <v>1</v>
-      </c>
-      <c r="D31" s="23">
-        <f>11/3.281</f>
-        <v>3.3526363913441024</v>
-      </c>
-      <c r="E31" s="24">
-        <f>8.25/3.281</f>
-        <v>2.5144772935080768</v>
-      </c>
-      <c r="F31" s="24">
-        <v>5.5E-2</v>
-      </c>
-      <c r="G31" s="36">
-        <f>PRODUCT(C31:F31)</f>
-        <v>0.46365704436829819</v>
-      </c>
+      <c r="B31" s="39"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="27"/>
       <c r="H31" s="25"/>
       <c r="I31" s="26"/>
       <c r="J31" s="27"/>
       <c r="K31" s="24"/>
     </row>
-    <row r="32" spans="1:15" s="1" customFormat="1">
-      <c r="A32" s="21"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="22">
-        <v>1</v>
-      </c>
-      <c r="D32" s="23">
-        <f>14.5/3.281</f>
-        <v>4.4193843340444987</v>
-      </c>
-      <c r="E32" s="24">
-        <f>10.25/3.281</f>
-        <v>3.1240475464797317</v>
-      </c>
-      <c r="F32" s="24">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="G32" s="36">
-        <f t="shared" ref="G32:G33" si="4">PRODUCT(C32:F32)</f>
-        <v>1.0354775089292008</v>
-      </c>
+    <row r="32" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A32" s="21">
+        <v>5</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="22"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="27"/>
       <c r="H32" s="25"/>
       <c r="I32" s="26"/>
       <c r="J32" s="27"/>
@@ -2369,25 +2369,26 @@
     </row>
     <row r="33" spans="1:31" s="1" customFormat="1">
       <c r="A33" s="21"/>
-      <c r="B33" s="39"/>
+      <c r="B33" s="39" t="s">
+        <v>35</v>
+      </c>
       <c r="C33" s="22">
-        <f t="shared" ref="C33:E33" si="5">C26</f>
         <v>1</v>
       </c>
       <c r="D33" s="23">
-        <f t="shared" si="5"/>
-        <v>4.5</v>
+        <f>11/3.281</f>
+        <v>3.3526363913441024</v>
       </c>
       <c r="E33" s="24">
-        <f t="shared" si="5"/>
-        <v>3.047851264858275</v>
+        <f>8.25/3.281</f>
+        <v>2.5144772935080768</v>
       </c>
       <c r="F33" s="24">
-        <v>7.4999999999999997E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="G33" s="36">
-        <f t="shared" si="4"/>
-        <v>1.0286498018896677</v>
+        <f>PRODUCT(C33:F33)</f>
+        <v>0.46365704436829819</v>
       </c>
       <c r="H33" s="25"/>
       <c r="I33" s="26"/>
@@ -2396,86 +2397,96 @@
     </row>
     <row r="34" spans="1:31" s="1" customFormat="1">
       <c r="A34" s="21"/>
-      <c r="B34" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="27">
-        <f>SUM(G31:G33)</f>
-        <v>2.5277843551871664</v>
-      </c>
-      <c r="H34" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="I34" s="26">
-        <v>12983.1</v>
-      </c>
-      <c r="J34" s="27">
-        <f>G34*I34</f>
-        <v>32818.477061830497</v>
-      </c>
+      <c r="B34" s="39"/>
+      <c r="C34" s="22">
+        <v>1</v>
+      </c>
+      <c r="D34" s="23">
+        <v>4.7</v>
+      </c>
+      <c r="E34" s="24">
+        <f>2.58</f>
+        <v>2.58</v>
+      </c>
+      <c r="F34" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="G34" s="36">
+        <f t="shared" ref="G34:G35" si="6">PRODUCT(C34:F34)</f>
+        <v>1.2126000000000001</v>
+      </c>
+      <c r="H34" s="25"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="27"/>
       <c r="K34" s="24"/>
     </row>
     <row r="35" spans="1:31" s="1" customFormat="1">
       <c r="A35" s="21"/>
-      <c r="B35" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="27"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="22">
+        <f t="shared" ref="C35:E35" si="7">C28</f>
+        <v>1</v>
+      </c>
+      <c r="D35" s="23">
+        <f>16/3.281</f>
+        <v>4.8765620237732392</v>
+      </c>
+      <c r="E35" s="24">
+        <f>(2.8+2.2)/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="F35" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="G35" s="36">
+        <f t="shared" si="6"/>
+        <v>1.2191405059433098</v>
+      </c>
       <c r="H35" s="25"/>
       <c r="I35" s="26"/>
-      <c r="J35" s="27">
-        <f>0.13*G34*8078.11</f>
-        <v>2654.5636100725301</v>
-      </c>
+      <c r="J35" s="27"/>
       <c r="K35" s="24"/>
     </row>
     <row r="36" spans="1:31" s="1" customFormat="1">
       <c r="A36" s="21"/>
-      <c r="B36" s="39"/>
+      <c r="B36" s="39" t="s">
+        <v>25</v>
+      </c>
       <c r="C36" s="22"/>
       <c r="D36" s="23"/>
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="27"/>
+      <c r="G36" s="27">
+        <f>SUM(G33:G35)</f>
+        <v>2.8953975503116078</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="I36" s="26">
+        <v>12983.1</v>
+      </c>
+      <c r="J36" s="27">
+        <f>G36*I36</f>
+        <v>37591.235935450633</v>
+      </c>
       <c r="K36" s="24"/>
     </row>
     <row r="37" spans="1:31" s="1" customFormat="1">
-      <c r="A37" s="21">
-        <v>6</v>
-      </c>
-      <c r="B37" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="22">
-        <v>1</v>
-      </c>
+      <c r="A37" s="21"/>
+      <c r="B37" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="22"/>
       <c r="D37" s="23"/>
       <c r="E37" s="24"/>
       <c r="F37" s="24"/>
-      <c r="G37" s="36">
-        <f>PRODUCT(C37:F37)</f>
-        <v>1</v>
-      </c>
-      <c r="H37" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="I37" s="26">
-        <v>500</v>
-      </c>
+      <c r="G37" s="27"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="26"/>
       <c r="J37" s="27">
-        <f>G37*I37</f>
-        <v>500</v>
+        <f>0.13*G36*8078.11</f>
+        <v>3040.6141876692013</v>
       </c>
       <c r="K37" s="24"/>
     </row>
@@ -2492,99 +2503,74 @@
       <c r="J38" s="27"/>
       <c r="K38" s="24"/>
     </row>
-    <row r="39" spans="1:31">
-      <c r="A39" s="9"/>
-      <c r="B39" s="20" t="s">
+    <row r="39" spans="1:31" s="1" customFormat="1">
+      <c r="A39" s="21">
+        <v>6</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="22">
+        <v>1</v>
+      </c>
+      <c r="D39" s="23"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="36">
+        <f>PRODUCT(C39:F39)</f>
+        <v>1</v>
+      </c>
+      <c r="H39" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="I39" s="26">
+        <v>500</v>
+      </c>
+      <c r="J39" s="27">
+        <f>G39*I39</f>
+        <v>500</v>
+      </c>
+      <c r="K39" s="24"/>
+    </row>
+    <row r="40" spans="1:31" s="1" customFormat="1">
+      <c r="A40" s="21"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="24"/>
+    </row>
+    <row r="41" spans="1:31">
+      <c r="A41" s="9"/>
+      <c r="B41" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7">
-        <f>SUM(J10:J38)</f>
-        <v>53534.943132230554</v>
-      </c>
-      <c r="K39" s="4"/>
-      <c r="M39" s="29"/>
-      <c r="P39" s="32"/>
-      <c r="Q39" s="32"/>
-    </row>
-    <row r="40" spans="1:31">
-      <c r="M40" s="29"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="31"/>
-      <c r="R40" s="30"/>
-      <c r="S40" s="30"/>
-      <c r="T40" s="30"/>
-      <c r="U40" s="29"/>
-      <c r="V40" s="29"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="29"/>
-      <c r="AC40" s="29"/>
-      <c r="AD40" s="29"/>
-      <c r="AE40" s="29"/>
-    </row>
-    <row r="41" spans="1:31" s="1" customFormat="1">
-      <c r="B41" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="75">
-        <f>J39</f>
-        <v>53534.943132230554</v>
-      </c>
-      <c r="D41" s="76"/>
-      <c r="E41" s="10">
-        <v>100</v>
-      </c>
-      <c r="F41" s="12"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="16"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="S41" s="30"/>
-      <c r="T41" s="30"/>
-      <c r="U41" s="12"/>
-      <c r="V41" s="12"/>
-      <c r="W41" s="12"/>
-      <c r="X41" s="12"/>
-      <c r="Y41" s="12"/>
-      <c r="Z41" s="12"/>
-      <c r="AA41" s="12"/>
-      <c r="AB41" s="12"/>
-      <c r="AC41" s="12"/>
-      <c r="AD41" s="12"/>
-      <c r="AE41" s="12"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7">
+        <f>SUM(J10:J40)</f>
+        <v>63819.543874106283</v>
+      </c>
+      <c r="K41" s="4"/>
+      <c r="M41" s="29"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
     </row>
     <row r="42" spans="1:31">
-      <c r="B42" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" s="79">
-        <v>60000</v>
-      </c>
-      <c r="D42" s="80"/>
-      <c r="E42" s="10"/>
       <c r="M42" s="29"/>
       <c r="N42" s="30"/>
       <c r="O42" s="30"/>
-      <c r="P42" s="30"/>
-      <c r="Q42" s="30"/>
+      <c r="P42" s="31"/>
       <c r="R42" s="30"/>
       <c r="S42" s="30"/>
       <c r="T42" s="30"/>
@@ -2600,59 +2586,61 @@
       <c r="AD42" s="29"/>
       <c r="AE42" s="29"/>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:31" s="1" customFormat="1">
       <c r="B43" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" s="79">
-        <v>30000</v>
-      </c>
-      <c r="D43" s="80"/>
+        <v>22</v>
+      </c>
+      <c r="C43" s="81">
+        <f>J41</f>
+        <v>63819.543874106283</v>
+      </c>
+      <c r="D43" s="82"/>
       <c r="E43" s="10">
-        <f>C43/C41*100</f>
-        <v>56.038165438787189</v>
-      </c>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29"/>
-      <c r="O43" s="29"/>
-      <c r="P43" s="29"/>
-      <c r="Q43" s="29"/>
-      <c r="R43" s="29"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="29"/>
-      <c r="U43" s="29"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="29"/>
-      <c r="Z43" s="29"/>
-      <c r="AA43" s="29"/>
-      <c r="AB43" s="29"/>
-      <c r="AC43" s="29"/>
-      <c r="AD43" s="29"/>
-      <c r="AE43" s="29"/>
+        <v>100</v>
+      </c>
+      <c r="F43" s="12"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="16"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="30"/>
+      <c r="O43" s="30"/>
+      <c r="P43" s="30"/>
+      <c r="Q43" s="30"/>
+      <c r="R43" s="30"/>
+      <c r="S43" s="30"/>
+      <c r="T43" s="30"/>
+      <c r="U43" s="12"/>
+      <c r="V43" s="12"/>
+      <c r="W43" s="12"/>
+      <c r="X43" s="12"/>
+      <c r="Y43" s="12"/>
+      <c r="Z43" s="12"/>
+      <c r="AA43" s="12"/>
+      <c r="AB43" s="12"/>
+      <c r="AC43" s="12"/>
+      <c r="AD43" s="12"/>
+      <c r="AE43" s="12"/>
     </row>
     <row r="44" spans="1:31">
       <c r="B44" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="81">
-        <f>C41-C43</f>
-        <v>23534.943132230554</v>
-      </c>
-      <c r="D44" s="81"/>
-      <c r="E44" s="10">
-        <f>100-E43</f>
-        <v>43.961834561212811</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C44" s="84">
+        <v>60000</v>
+      </c>
+      <c r="D44" s="85"/>
+      <c r="E44" s="10"/>
       <c r="M44" s="29"/>
-      <c r="N44" s="29"/>
-      <c r="O44" s="29"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
+      <c r="N44" s="30"/>
+      <c r="O44" s="30"/>
+      <c r="P44" s="30"/>
+      <c r="Q44" s="30"/>
+      <c r="R44" s="30"/>
+      <c r="S44" s="30"/>
+      <c r="T44" s="30"/>
       <c r="U44" s="29"/>
       <c r="V44" s="29"/>
       <c r="W44" s="29"/>
@@ -2667,15 +2655,15 @@
     </row>
     <row r="45" spans="1:31">
       <c r="B45" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C45" s="75">
-        <f>C42*0.03</f>
-        <v>1800</v>
-      </c>
-      <c r="D45" s="76"/>
+        <v>18</v>
+      </c>
+      <c r="C45" s="84">
+        <v>30000</v>
+      </c>
+      <c r="D45" s="85"/>
       <c r="E45" s="10">
-        <v>3</v>
+        <f>C45/C43*100</f>
+        <v>47.007543737980242</v>
       </c>
       <c r="M45" s="29"/>
       <c r="N45" s="29"/>
@@ -2699,15 +2687,16 @@
     </row>
     <row r="46" spans="1:31">
       <c r="B46" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C46" s="75">
-        <f>C42*0.02</f>
-        <v>1200</v>
-      </c>
-      <c r="D46" s="76"/>
+        <v>19</v>
+      </c>
+      <c r="C46" s="86">
+        <f>C43-C45</f>
+        <v>33819.543874106283</v>
+      </c>
+      <c r="D46" s="86"/>
       <c r="E46" s="10">
-        <v>2</v>
+        <f>100-E45</f>
+        <v>52.992456262019758</v>
       </c>
       <c r="M46" s="29"/>
       <c r="N46" s="29"/>
@@ -2729,8 +2718,80 @@
       <c r="AD46" s="29"/>
       <c r="AE46" s="29"/>
     </row>
+    <row r="47" spans="1:31">
+      <c r="B47" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="81">
+        <f>C44*0.03</f>
+        <v>1800</v>
+      </c>
+      <c r="D47" s="82"/>
+      <c r="E47" s="10">
+        <v>3</v>
+      </c>
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
+      <c r="O47" s="29"/>
+      <c r="P47" s="29"/>
+      <c r="Q47" s="29"/>
+      <c r="R47" s="29"/>
+      <c r="S47" s="29"/>
+      <c r="T47" s="29"/>
+      <c r="U47" s="29"/>
+      <c r="V47" s="29"/>
+      <c r="W47" s="29"/>
+      <c r="X47" s="29"/>
+      <c r="Y47" s="29"/>
+      <c r="Z47" s="29"/>
+      <c r="AA47" s="29"/>
+      <c r="AB47" s="29"/>
+      <c r="AC47" s="29"/>
+      <c r="AD47" s="29"/>
+      <c r="AE47" s="29"/>
+    </row>
+    <row r="48" spans="1:31">
+      <c r="B48" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="81">
+        <f>C44*0.02</f>
+        <v>1200</v>
+      </c>
+      <c r="D48" s="82"/>
+      <c r="E48" s="10">
+        <v>2</v>
+      </c>
+      <c r="M48" s="29"/>
+      <c r="N48" s="29"/>
+      <c r="O48" s="29"/>
+      <c r="P48" s="29"/>
+      <c r="Q48" s="29"/>
+      <c r="R48" s="29"/>
+      <c r="S48" s="29"/>
+      <c r="T48" s="29"/>
+      <c r="U48" s="29"/>
+      <c r="V48" s="29"/>
+      <c r="W48" s="29"/>
+      <c r="X48" s="29"/>
+      <c r="Y48" s="29"/>
+      <c r="Z48" s="29"/>
+      <c r="AA48" s="29"/>
+      <c r="AB48" s="29"/>
+      <c r="AC48" s="29"/>
+      <c r="AD48" s="29"/>
+      <c r="AE48" s="29"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -2738,14 +2799,6 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2764,18 +2817,18 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="43" customFormat="1" ht="20.100000000000001" customHeight="1">
@@ -2875,7 +2928,7 @@
         <v>2497.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="43" customFormat="1" ht="16.2">
+    <row r="6" spans="1:8" s="43" customFormat="1" ht="16.5">
       <c r="B6" s="93" t="s">
         <v>52</v>
       </c>
@@ -2898,7 +2951,7 @@
       </c>
       <c r="H6" s="59"/>
     </row>
-    <row r="7" spans="1:8" s="43" customFormat="1" ht="16.2">
+    <row r="7" spans="1:8" s="43" customFormat="1" ht="16.5">
       <c r="B7" s="94"/>
       <c r="C7" s="57" t="s">
         <v>54</v>
@@ -3016,7 +3069,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="43" customFormat="1" ht="15">
+    <row r="14" spans="1:8" s="43" customFormat="1">
       <c r="A14" s="73" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
estimate given to pashu shakha
</commit_message>
<xml_diff>
--- a/ofc/पशु शाखा इस्तिमेट/kamal.xlsx
+++ b/ofc/पशु शाखा इस्तिमेट/kamal.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="as per mistry" sheetId="19" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="20" r:id="rId2"/>
+    <sheet name="field" sheetId="19" state="hidden" r:id="rId1"/>
+    <sheet name="as per mistry (2)" sheetId="21" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="20" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="_cgi24">'[1]update Rate'!$N$95</definedName>
@@ -43,8 +44,10 @@
     <definedName name="description_784">[3]Abstract!$B$300</definedName>
     <definedName name="excavator">[2]Equipment_Rate!$J$19</definedName>
     <definedName name="generator">[2]Equipment_Rate!$J$20</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'as per mistry'!$A$1:$K$48</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'as per mistry'!$1:$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'as per mistry (2)'!$A$1:$K$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">field!$A$1:$K$50</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'as per mistry (2)'!$1:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">field!$1:$8</definedName>
     <definedName name="skilled">[2]District_Rate!$D$148</definedName>
     <definedName name="skilled_blacksmith">[2]District_Rate!$D$149</definedName>
     <definedName name="unskilled">[2]District_Rate!$D$156</definedName>
@@ -59,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="76">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -288,6 +291,33 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">)=@$ dL=dL= afSnf] ;L=hL=cfO{= 5fgf 5fpg] sfd </t>
+  </si>
+  <si>
+    <t>-for passage flooring</t>
+  </si>
+  <si>
+    <t>Project:- फ्रेंश कृषि तथा पशुपालन</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date: 2082/02/05  </t>
+  </si>
+  <si>
+    <t>husf] vf8ndf 9'+uf eg]{ / n]en ug]{ sfddf</t>
+  </si>
+  <si>
+    <t>-MS square pipe of 1.5"*1.5" of 1.6mm thickness</t>
+  </si>
+  <si>
+    <t>Project:- इन्द्रायणी एग्रो फर्म प्रा. लि .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date:                     </t>
+  </si>
+  <si>
+    <t>dfn;fdfg pknAw u/L )=१७ dL=dL= afSnf] ;L=hL=cfO{= zL6 -h:tf kftfsf]_ 5fgf 5fpg] sfd k'/f .</t>
+  </si>
+  <si>
     <r>
       <t>CGI</t>
     </r>
@@ -311,29 +341,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>(0.24mm)</t>
+      <t>(0.१७mm)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">)=@$ dL=dL= afSnf] ;L=hL=cfO{= 5fgf 5fpg] sfd </t>
-  </si>
-  <si>
-    <t>-for passage flooring</t>
-  </si>
-  <si>
-    <t>Project:- फ्रेंश कृषि तथा पशुपालन</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date: 2082/02/05  </t>
-  </si>
-  <si>
-    <t>husf] vf8ndf 9'+uf eg]{ / n]en ug]{ sfddf</t>
-  </si>
-  <si>
-    <t>dfn;fdfg pknAw u/L )=@$ dL=dL= afSnf] ;L=hL=cfO{= zL6 -h:tf kftfsf]_ 5fgf 5fpg] sfd k'/f .</t>
-  </si>
-  <si>
-    <t>-MS square pipe of 1.5"*1.5" of 1.6mm thickness</t>
+    <t xml:space="preserve">;L=hL=cfO{= 5fgf 5fpg] sfd </t>
   </si>
 </sst>
 </file>
@@ -505,7 +517,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -620,6 +632,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -631,7 +654,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -879,6 +902,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1666,10 +1701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE48"/>
+  <dimension ref="A1:AE50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1768,7 +1803,7 @@
     </row>
     <row r="6" spans="1:13" ht="18.75">
       <c r="A6" s="75" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="75"/>
       <c r="C6" s="75"/>
@@ -1794,7 +1829,7 @@
       <c r="F7" s="83"/>
       <c r="G7" s="2"/>
       <c r="H7" s="76" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I7" s="76"/>
       <c r="J7" s="76"/>
@@ -1863,7 +1898,7 @@
     <row r="10" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A10" s="38"/>
       <c r="B10" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" s="40">
         <v>3</v>
@@ -1998,167 +2033,195 @@
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" s="1" customFormat="1">
-      <c r="A15" s="21"/>
-      <c r="B15" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="27">
-        <f>SUM(G10:G14)</f>
-        <v>47.82832633343493</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I15" s="26">
-        <v>181.17</v>
-      </c>
-      <c r="J15" s="27">
-        <f>G15*I15</f>
-        <v>8665.0578818284048</v>
-      </c>
-      <c r="K15" s="24"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="40">
+        <v>3</v>
+      </c>
+      <c r="D15" s="10">
+        <f>7/3.281</f>
+        <v>2.1334958854007922</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1.83</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" ref="F15" si="4">PRODUCT(C15:E15)</f>
+        <v>11.712892410850349</v>
+      </c>
+      <c r="G15" s="36">
+        <f t="shared" ref="G15" si="5">F15</f>
+        <v>11.712892410850349</v>
+      </c>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="11"/>
+      <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:13" s="1" customFormat="1">
-      <c r="A16" s="21"/>
-      <c r="B16" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27">
-        <f>0.13*G15*(1871.42/18.94)</f>
-        <v>614.35560932941837</v>
-      </c>
-      <c r="K16" s="24"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40">
+        <v>2</v>
+      </c>
+      <c r="D16" s="10">
+        <f>4.5</f>
+        <v>4.5</v>
+      </c>
+      <c r="E16" s="10">
+        <v>1.83</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" ref="F16" si="6">PRODUCT(C16:E16)</f>
+        <v>16.47</v>
+      </c>
+      <c r="G16" s="36">
+        <f t="shared" ref="G16" si="7">F16</f>
+        <v>16.47</v>
+      </c>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="11"/>
+      <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:15" s="1" customFormat="1">
       <c r="A17" s="21"/>
-      <c r="B17" s="37"/>
+      <c r="B17" s="39" t="s">
+        <v>25</v>
+      </c>
       <c r="C17" s="22"/>
       <c r="D17" s="23"/>
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27"/>
+      <c r="G17" s="27">
+        <f>SUM(G10:G16)</f>
+        <v>76.011218744285287</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="26">
+        <v>181.17</v>
+      </c>
+      <c r="J17" s="27">
+        <f>G17*I17</f>
+        <v>13770.952499902165</v>
+      </c>
       <c r="K17" s="24"/>
     </row>
-    <row r="18" spans="1:15" s="1" customFormat="1" ht="30">
-      <c r="A18" s="38">
+    <row r="18" spans="1:15" s="1" customFormat="1">
+      <c r="A18" s="21"/>
+      <c r="B18" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27">
+        <f>0.13*G17*(1871.42/18.94)</f>
+        <v>976.36530874952211</v>
+      </c>
+      <c r="K18" s="24"/>
+    </row>
+    <row r="19" spans="1:15" s="1" customFormat="1">
+      <c r="A19" s="21"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A20" s="38">
         <v>2</v>
       </c>
-      <c r="B18" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="11"/>
-      <c r="M18" s="12"/>
-    </row>
-    <row r="19" spans="1:15" s="1" customFormat="1">
-      <c r="A19" s="38"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40">
-        <v>5</v>
-      </c>
-      <c r="D19" s="10">
-        <f>8/3.281</f>
-        <v>2.4382810118866196</v>
-      </c>
-      <c r="E19" s="10">
-        <f>2.17/3.281</f>
-        <v>0.66138372447424565</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="36">
-        <f>PRODUCT(C19:F19)</f>
-        <v>8.063196884782025</v>
-      </c>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="11"/>
-      <c r="M19" s="12"/>
-    </row>
-    <row r="20" spans="1:15" s="1" customFormat="1">
-      <c r="A20" s="21"/>
-      <c r="B20" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="27">
-        <f>SUM(G19:G19)</f>
-        <v>8.063196884782025</v>
-      </c>
-      <c r="H20" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="I20" s="26">
-        <f>Sheet1!H10/10</f>
-        <v>249.75</v>
-      </c>
-      <c r="J20" s="27">
-        <f>G20*I20</f>
-        <v>2013.7834219743108</v>
-      </c>
-      <c r="K20" s="24"/>
+      <c r="B20" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="40"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="11"/>
+      <c r="M20" s="12"/>
     </row>
     <row r="21" spans="1:15" s="1" customFormat="1">
-      <c r="A21" s="21"/>
-      <c r="B21" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="27">
-        <f>0*0.13*G20*5298.54/10</f>
-        <v>0</v>
-      </c>
-      <c r="K21" s="24"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="40">
+        <v>1</v>
+      </c>
+      <c r="D21" s="10">
+        <v>4</v>
+      </c>
+      <c r="E21" s="10">
+        <f>7/3.281</f>
+        <v>2.1334958854007922</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="36">
+        <f>PRODUCT(C21:F21)</f>
+        <v>8.5339835416031686</v>
+      </c>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="11"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="1">
+        <f>D21*5</f>
+        <v>20</v>
+      </c>
+      <c r="O21" s="1">
+        <f>4.5</f>
+        <v>4.5</v>
+      </c>
     </row>
     <row r="22" spans="1:15" s="1" customFormat="1">
       <c r="A22" s="21"/>
-      <c r="B22" s="39"/>
+      <c r="B22" s="39" t="s">
+        <v>25</v>
+      </c>
       <c r="C22" s="22"/>
       <c r="D22" s="23"/>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="27"/>
+      <c r="G22" s="27">
+        <f>SUM(G21:G21)</f>
+        <v>8.5339835416031686</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="26">
+        <f>Sheet1!H10/10</f>
+        <v>249.75</v>
+      </c>
+      <c r="J22" s="27">
+        <f>G22*I22</f>
+        <v>2131.3623895153914</v>
+      </c>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="1:15" s="1" customFormat="1" ht="30">
-      <c r="A23" s="21">
-        <v>3</v>
-      </c>
-      <c r="B23" s="37" t="s">
-        <v>34</v>
+    <row r="23" spans="1:15" s="1" customFormat="1" hidden="1">
+      <c r="A23" s="21"/>
+      <c r="B23" s="39" t="s">
+        <v>33</v>
       </c>
       <c r="C23" s="22"/>
       <c r="D23" s="23"/>
@@ -2167,195 +2230,181 @@
       <c r="G23" s="27"/>
       <c r="H23" s="25"/>
       <c r="I23" s="26"/>
-      <c r="J23" s="27"/>
+      <c r="J23" s="27">
+        <f>0*0.13*G22*5298.54/10</f>
+        <v>0</v>
+      </c>
       <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:15" s="1" customFormat="1">
       <c r="A24" s="21"/>
-      <c r="B24" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="22">
-        <v>1</v>
-      </c>
-      <c r="D24" s="23">
-        <v>4.5</v>
-      </c>
-      <c r="E24" s="24">
-        <f>10/3.281</f>
-        <v>3.047851264858275</v>
-      </c>
-      <c r="F24" s="24">
-        <v>0.15</v>
-      </c>
-      <c r="G24" s="36">
-        <f t="shared" ref="G24" si="4">PRODUCT(C24:F24)</f>
-        <v>2.0572996037793354</v>
-      </c>
+      <c r="B24" s="39"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="27"/>
       <c r="H24" s="25"/>
       <c r="I24" s="26"/>
       <c r="J24" s="27"/>
       <c r="K24" s="24"/>
     </row>
-    <row r="25" spans="1:15" s="1" customFormat="1">
-      <c r="A25" s="21"/>
-      <c r="B25" s="39" t="s">
-        <v>25</v>
+    <row r="25" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A25" s="21">
+        <v>3</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>34</v>
       </c>
       <c r="C25" s="22"/>
       <c r="D25" s="23"/>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
-      <c r="G25" s="27">
-        <f>SUM(G24:G24)</f>
-        <v>2.0572996037793354</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="I25" s="26">
-        <v>663.31</v>
-      </c>
-      <c r="J25" s="27">
-        <f>G25*I25</f>
-        <v>1364.6274001828708</v>
-      </c>
+      <c r="G25" s="27"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
       <c r="K25" s="24"/>
     </row>
     <row r="26" spans="1:15" s="1" customFormat="1">
       <c r="A26" s="21"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="27"/>
+      <c r="B26" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="22">
+        <v>1</v>
+      </c>
+      <c r="D26" s="23">
+        <f>D37</f>
+        <v>4.8765620237732392</v>
+      </c>
+      <c r="E26" s="24">
+        <f>10/3.281</f>
+        <v>3.047851264858275</v>
+      </c>
+      <c r="F26" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="G26" s="36">
+        <f t="shared" ref="G26" si="8">PRODUCT(C26:F26)</f>
+        <v>2.2294553598475644</v>
+      </c>
       <c r="H26" s="25"/>
       <c r="I26" s="26"/>
       <c r="J26" s="27"/>
       <c r="K26" s="24"/>
     </row>
-    <row r="27" spans="1:15" s="1" customFormat="1" ht="30">
-      <c r="A27" s="21">
-        <v>4</v>
-      </c>
-      <c r="B27" s="74" t="s">
-        <v>70</v>
+    <row r="27" spans="1:15" s="1" customFormat="1">
+      <c r="A27" s="21"/>
+      <c r="B27" s="39" t="s">
+        <v>25</v>
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="23"/>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="27"/>
+      <c r="G27" s="27">
+        <f>SUM(G26:G26)</f>
+        <v>2.2294553598475644</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="26">
+        <v>663.31</v>
+      </c>
+      <c r="J27" s="27">
+        <f>G27*I27</f>
+        <v>1478.8200347404877</v>
+      </c>
       <c r="K27" s="24"/>
     </row>
     <row r="28" spans="1:15" s="1" customFormat="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="39" t="str">
-        <f>B24</f>
-        <v>-for passage flooring</v>
-      </c>
-      <c r="C28" s="22">
-        <f>C24</f>
-        <v>1</v>
-      </c>
-      <c r="D28" s="23">
-        <f>D24</f>
-        <v>4.5</v>
-      </c>
-      <c r="E28" s="24">
-        <f>10/3.281</f>
-        <v>3.047851264858275</v>
-      </c>
-      <c r="F28" s="24">
-        <v>0.15</v>
-      </c>
-      <c r="G28" s="36">
-        <f t="shared" ref="G28" si="5">PRODUCT(C28:F28)</f>
-        <v>2.0572996037793354</v>
-      </c>
+      <c r="B28" s="39"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="27"/>
       <c r="H28" s="25"/>
       <c r="I28" s="26"/>
       <c r="J28" s="27"/>
       <c r="K28" s="24"/>
     </row>
-    <row r="29" spans="1:15" s="1" customFormat="1">
-      <c r="A29" s="21"/>
-      <c r="B29" s="39" t="s">
-        <v>25</v>
+    <row r="29" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A29" s="21">
+        <v>4</v>
+      </c>
+      <c r="B29" s="74" t="s">
+        <v>69</v>
       </c>
       <c r="C29" s="22"/>
       <c r="D29" s="23"/>
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
-      <c r="G29" s="27">
-        <f>SUM(G28:G28)</f>
-        <v>2.0572996037793354</v>
-      </c>
-      <c r="H29" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" s="26">
-        <v>4473.1499999999996</v>
-      </c>
-      <c r="J29" s="27">
-        <f>G29*I29</f>
-        <v>9202.6097226455331</v>
-      </c>
+      <c r="G29" s="27"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="27"/>
       <c r="K29" s="24"/>
     </row>
     <row r="30" spans="1:15" s="1" customFormat="1">
       <c r="A30" s="21"/>
-      <c r="B30" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="27"/>
+      <c r="B30" s="39" t="str">
+        <f>B26</f>
+        <v>-for passage flooring</v>
+      </c>
+      <c r="C30" s="22">
+        <v>1</v>
+      </c>
+      <c r="D30" s="23">
+        <v>4</v>
+      </c>
+      <c r="E30" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="F30" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="G30" s="36">
+        <f t="shared" ref="G30" si="9">PRODUCT(C30:F30)</f>
+        <v>0.89999999999999991</v>
+      </c>
       <c r="H30" s="25"/>
       <c r="I30" s="26"/>
-      <c r="J30" s="27">
-        <f>0.13*G29*3093.15</f>
-        <v>827.25971502590676</v>
-      </c>
+      <c r="J30" s="27"/>
       <c r="K30" s="24"/>
-      <c r="M30" s="1">
-        <f>4434</f>
-        <v>4434</v>
-      </c>
-      <c r="N30" s="1" t="e">
-        <f>(PRODUCT(#REF!))*0.15+(PRODUCT(#REF!))*0.15+(PRODUCT(C28:E28))*0.15</f>
-        <v>#REF!</v>
-      </c>
-      <c r="O30" s="1" t="e">
-        <f>N30*M30</f>
-        <v>#REF!</v>
-      </c>
     </row>
     <row r="31" spans="1:15" s="1" customFormat="1">
       <c r="A31" s="21"/>
-      <c r="B31" s="39"/>
+      <c r="B31" s="39" t="s">
+        <v>25</v>
+      </c>
       <c r="C31" s="22"/>
       <c r="D31" s="23"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="27"/>
+      <c r="G31" s="27">
+        <f>SUM(G30:G30)</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="26">
+        <v>4473.1499999999996</v>
+      </c>
+      <c r="J31" s="27">
+        <f>G31*I31</f>
+        <v>4025.8349999999991</v>
+      </c>
       <c r="K31" s="24"/>
     </row>
-    <row r="32" spans="1:15" s="1" customFormat="1" ht="30">
-      <c r="A32" s="21">
-        <v>5</v>
-      </c>
-      <c r="B32" s="37" t="s">
-        <v>37</v>
+    <row r="32" spans="1:15" s="1" customFormat="1">
+      <c r="A32" s="21"/>
+      <c r="B32" s="39" t="s">
+        <v>33</v>
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="23"/>
@@ -2364,57 +2413,49 @@
       <c r="G32" s="27"/>
       <c r="H32" s="25"/>
       <c r="I32" s="26"/>
-      <c r="J32" s="27"/>
+      <c r="J32" s="27">
+        <f>0.13*G31*3093.15</f>
+        <v>361.89855</v>
+      </c>
       <c r="K32" s="24"/>
+      <c r="M32" s="1">
+        <f>4434</f>
+        <v>4434</v>
+      </c>
+      <c r="N32" s="1" t="e">
+        <f>(PRODUCT(#REF!))*0.15+(PRODUCT(#REF!))*0.15+(PRODUCT(C30:E30))*0.15</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O32" s="1" t="e">
+        <f>N32*M32</f>
+        <v>#REF!</v>
+      </c>
     </row>
     <row r="33" spans="1:31" s="1" customFormat="1">
       <c r="A33" s="21"/>
-      <c r="B33" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="22">
-        <v>1</v>
-      </c>
-      <c r="D33" s="23">
-        <f>11/3.281</f>
-        <v>3.3526363913441024</v>
-      </c>
-      <c r="E33" s="24">
-        <f>8.25/3.281</f>
-        <v>2.5144772935080768</v>
-      </c>
-      <c r="F33" s="24">
-        <v>5.5E-2</v>
-      </c>
-      <c r="G33" s="36">
-        <f>PRODUCT(C33:F33)</f>
-        <v>0.46365704436829819</v>
-      </c>
+      <c r="B33" s="39"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="27"/>
       <c r="H33" s="25"/>
       <c r="I33" s="26"/>
       <c r="J33" s="27"/>
       <c r="K33" s="24"/>
     </row>
-    <row r="34" spans="1:31" s="1" customFormat="1">
-      <c r="A34" s="21"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="22">
-        <v>1</v>
-      </c>
-      <c r="D34" s="23">
-        <v>4.7</v>
-      </c>
-      <c r="E34" s="24">
-        <f>2.58</f>
-        <v>2.58</v>
-      </c>
-      <c r="F34" s="24">
-        <v>0.1</v>
-      </c>
-      <c r="G34" s="36">
-        <f t="shared" ref="G34:G35" si="6">PRODUCT(C34:F34)</f>
-        <v>1.2126000000000001</v>
-      </c>
+    <row r="34" spans="1:31" s="1" customFormat="1" ht="30">
+      <c r="A34" s="21">
+        <v>5</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="27"/>
       <c r="H34" s="25"/>
       <c r="I34" s="26"/>
       <c r="J34" s="27"/>
@@ -2422,25 +2463,26 @@
     </row>
     <row r="35" spans="1:31" s="1" customFormat="1">
       <c r="A35" s="21"/>
-      <c r="B35" s="39"/>
+      <c r="B35" s="39" t="s">
+        <v>35</v>
+      </c>
       <c r="C35" s="22">
-        <f t="shared" ref="C35:E35" si="7">C28</f>
         <v>1</v>
       </c>
       <c r="D35" s="23">
-        <f>16/3.281</f>
-        <v>4.8765620237732392</v>
+        <f>11/3.281</f>
+        <v>3.3526363913441024</v>
       </c>
       <c r="E35" s="24">
-        <f>(2.8+2.2)/2</f>
-        <v>2.5</v>
+        <f>8.25/3.281</f>
+        <v>2.5144772935080768</v>
       </c>
       <c r="F35" s="24">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G35" s="36">
-        <f t="shared" si="6"/>
-        <v>1.2191405059433098</v>
+        <f>PRODUCT(C35:F35)</f>
+        <v>0.42150640397118022</v>
       </c>
       <c r="H35" s="25"/>
       <c r="I35" s="26"/>
@@ -2449,86 +2491,95 @@
     </row>
     <row r="36" spans="1:31" s="1" customFormat="1">
       <c r="A36" s="21"/>
-      <c r="B36" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" s="22"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="27">
-        <f>SUM(G33:G35)</f>
-        <v>2.8953975503116078</v>
-      </c>
-      <c r="H36" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="I36" s="26">
-        <v>12983.1</v>
-      </c>
-      <c r="J36" s="27">
-        <f>G36*I36</f>
-        <v>37591.235935450633</v>
-      </c>
+      <c r="B36" s="39"/>
+      <c r="C36" s="22">
+        <v>1</v>
+      </c>
+      <c r="D36" s="23">
+        <v>4.7</v>
+      </c>
+      <c r="E36" s="24">
+        <f>2.58</f>
+        <v>2.58</v>
+      </c>
+      <c r="F36" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="G36" s="36">
+        <f t="shared" ref="G36:G37" si="10">PRODUCT(C36:F36)</f>
+        <v>1.2126000000000001</v>
+      </c>
+      <c r="H36" s="25"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="27"/>
       <c r="K36" s="24"/>
     </row>
     <row r="37" spans="1:31" s="1" customFormat="1">
       <c r="A37" s="21"/>
-      <c r="B37" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="27"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="22">
+        <v>1</v>
+      </c>
+      <c r="D37" s="23">
+        <f>16/3.281</f>
+        <v>4.8765620237732392</v>
+      </c>
+      <c r="E37" s="24">
+        <f>(2.8+2.2)/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="F37" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="G37" s="36">
+        <f t="shared" si="10"/>
+        <v>1.2191405059433098</v>
+      </c>
       <c r="H37" s="25"/>
       <c r="I37" s="26"/>
-      <c r="J37" s="27">
-        <f>0.13*G36*8078.11</f>
-        <v>3040.6141876692013</v>
-      </c>
+      <c r="J37" s="27"/>
       <c r="K37" s="24"/>
     </row>
     <row r="38" spans="1:31" s="1" customFormat="1">
       <c r="A38" s="21"/>
-      <c r="B38" s="39"/>
+      <c r="B38" s="39" t="s">
+        <v>25</v>
+      </c>
       <c r="C38" s="22"/>
       <c r="D38" s="23"/>
       <c r="E38" s="24"/>
       <c r="F38" s="24"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="27"/>
+      <c r="G38" s="27">
+        <f>SUM(G35:G37)</f>
+        <v>2.8532469099144899</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="I38" s="26">
+        <v>12983.1</v>
+      </c>
+      <c r="J38" s="27">
+        <f>G38*I38</f>
+        <v>37043.989956110818</v>
+      </c>
       <c r="K38" s="24"/>
     </row>
     <row r="39" spans="1:31" s="1" customFormat="1">
-      <c r="A39" s="21">
-        <v>6</v>
-      </c>
-      <c r="B39" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="22">
-        <v>1</v>
-      </c>
+      <c r="A39" s="21"/>
+      <c r="B39" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="22"/>
       <c r="D39" s="23"/>
       <c r="E39" s="24"/>
       <c r="F39" s="24"/>
-      <c r="G39" s="36">
-        <f>PRODUCT(C39:F39)</f>
-        <v>1</v>
-      </c>
-      <c r="H39" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="I39" s="26">
-        <v>500</v>
-      </c>
+      <c r="G39" s="27"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="26"/>
       <c r="J39" s="27">
-        <f>G39*I39</f>
-        <v>500</v>
+        <f>0.13*G38*8078.11</f>
+        <v>2996.3495114084144</v>
       </c>
       <c r="K39" s="24"/>
     </row>
@@ -2545,99 +2596,74 @@
       <c r="J40" s="27"/>
       <c r="K40" s="24"/>
     </row>
-    <row r="41" spans="1:31">
-      <c r="A41" s="9"/>
-      <c r="B41" s="20" t="s">
+    <row r="41" spans="1:31" s="1" customFormat="1">
+      <c r="A41" s="21">
+        <v>6</v>
+      </c>
+      <c r="B41" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="22">
+        <v>1</v>
+      </c>
+      <c r="D41" s="23"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="36">
+        <f>PRODUCT(C41:F41)</f>
+        <v>1</v>
+      </c>
+      <c r="H41" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="I41" s="26">
+        <v>500</v>
+      </c>
+      <c r="J41" s="27">
+        <f>G41*I41</f>
+        <v>500</v>
+      </c>
+      <c r="K41" s="24"/>
+    </row>
+    <row r="42" spans="1:31" s="1" customFormat="1">
+      <c r="A42" s="21"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="24"/>
+    </row>
+    <row r="43" spans="1:31">
+      <c r="A43" s="9"/>
+      <c r="B43" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7">
-        <f>SUM(J10:J40)</f>
-        <v>63819.543874106283</v>
-      </c>
-      <c r="K41" s="4"/>
-      <c r="M41" s="29"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
-    </row>
-    <row r="42" spans="1:31">
-      <c r="M42" s="29"/>
-      <c r="N42" s="30"/>
-      <c r="O42" s="30"/>
-      <c r="P42" s="31"/>
-      <c r="R42" s="30"/>
-      <c r="S42" s="30"/>
-      <c r="T42" s="30"/>
-      <c r="U42" s="29"/>
-      <c r="V42" s="29"/>
-      <c r="W42" s="29"/>
-      <c r="X42" s="29"/>
-      <c r="Y42" s="29"/>
-      <c r="Z42" s="29"/>
-      <c r="AA42" s="29"/>
-      <c r="AB42" s="29"/>
-      <c r="AC42" s="29"/>
-      <c r="AD42" s="29"/>
-      <c r="AE42" s="29"/>
-    </row>
-    <row r="43" spans="1:31" s="1" customFormat="1">
-      <c r="B43" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C43" s="81">
-        <f>J41</f>
-        <v>63819.543874106283</v>
-      </c>
-      <c r="D43" s="82"/>
-      <c r="E43" s="10">
-        <v>100</v>
-      </c>
-      <c r="F43" s="12"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="16"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="30"/>
-      <c r="O43" s="30"/>
-      <c r="P43" s="30"/>
-      <c r="Q43" s="30"/>
-      <c r="R43" s="30"/>
-      <c r="S43" s="30"/>
-      <c r="T43" s="30"/>
-      <c r="U43" s="12"/>
-      <c r="V43" s="12"/>
-      <c r="W43" s="12"/>
-      <c r="X43" s="12"/>
-      <c r="Y43" s="12"/>
-      <c r="Z43" s="12"/>
-      <c r="AA43" s="12"/>
-      <c r="AB43" s="12"/>
-      <c r="AC43" s="12"/>
-      <c r="AD43" s="12"/>
-      <c r="AE43" s="12"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7">
+        <f>SUM(J10:J42)</f>
+        <v>63285.573250426802</v>
+      </c>
+      <c r="K43" s="4"/>
+      <c r="M43" s="29"/>
+      <c r="P43" s="32"/>
+      <c r="Q43" s="32"/>
     </row>
     <row r="44" spans="1:31">
-      <c r="B44" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" s="84">
-        <v>60000</v>
-      </c>
-      <c r="D44" s="85"/>
-      <c r="E44" s="10"/>
       <c r="M44" s="29"/>
       <c r="N44" s="30"/>
       <c r="O44" s="30"/>
-      <c r="P44" s="30"/>
-      <c r="Q44" s="30"/>
+      <c r="P44" s="31"/>
       <c r="R44" s="30"/>
       <c r="S44" s="30"/>
       <c r="T44" s="30"/>
@@ -2653,59 +2679,61 @@
       <c r="AD44" s="29"/>
       <c r="AE44" s="29"/>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:31" s="1" customFormat="1">
       <c r="B45" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C45" s="84">
-        <v>30000</v>
-      </c>
-      <c r="D45" s="85"/>
+        <v>22</v>
+      </c>
+      <c r="C45" s="81">
+        <f>J43</f>
+        <v>63285.573250426802</v>
+      </c>
+      <c r="D45" s="82"/>
       <c r="E45" s="10">
-        <f>C45/C43*100</f>
-        <v>47.007543737980242</v>
-      </c>
-      <c r="M45" s="29"/>
-      <c r="N45" s="29"/>
-      <c r="O45" s="29"/>
-      <c r="P45" s="29"/>
-      <c r="Q45" s="29"/>
-      <c r="R45" s="29"/>
-      <c r="S45" s="29"/>
-      <c r="T45" s="29"/>
-      <c r="U45" s="29"/>
-      <c r="V45" s="29"/>
-      <c r="W45" s="29"/>
-      <c r="X45" s="29"/>
-      <c r="Y45" s="29"/>
-      <c r="Z45" s="29"/>
-      <c r="AA45" s="29"/>
-      <c r="AB45" s="29"/>
-      <c r="AC45" s="29"/>
-      <c r="AD45" s="29"/>
-      <c r="AE45" s="29"/>
+        <v>100</v>
+      </c>
+      <c r="F45" s="12"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="16"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="30"/>
+      <c r="O45" s="30"/>
+      <c r="P45" s="30"/>
+      <c r="Q45" s="30"/>
+      <c r="R45" s="30"/>
+      <c r="S45" s="30"/>
+      <c r="T45" s="30"/>
+      <c r="U45" s="12"/>
+      <c r="V45" s="12"/>
+      <c r="W45" s="12"/>
+      <c r="X45" s="12"/>
+      <c r="Y45" s="12"/>
+      <c r="Z45" s="12"/>
+      <c r="AA45" s="12"/>
+      <c r="AB45" s="12"/>
+      <c r="AC45" s="12"/>
+      <c r="AD45" s="12"/>
+      <c r="AE45" s="12"/>
     </row>
     <row r="46" spans="1:31">
       <c r="B46" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" s="86">
-        <f>C43-C45</f>
-        <v>33819.543874106283</v>
-      </c>
-      <c r="D46" s="86"/>
-      <c r="E46" s="10">
-        <f>100-E45</f>
-        <v>52.992456262019758</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C46" s="84">
+        <v>60000</v>
+      </c>
+      <c r="D46" s="85"/>
+      <c r="E46" s="10"/>
       <c r="M46" s="29"/>
-      <c r="N46" s="29"/>
-      <c r="O46" s="29"/>
-      <c r="P46" s="29"/>
-      <c r="Q46" s="29"/>
-      <c r="R46" s="29"/>
-      <c r="S46" s="29"/>
-      <c r="T46" s="29"/>
+      <c r="N46" s="30"/>
+      <c r="O46" s="30"/>
+      <c r="P46" s="30"/>
+      <c r="Q46" s="30"/>
+      <c r="R46" s="30"/>
+      <c r="S46" s="30"/>
+      <c r="T46" s="30"/>
       <c r="U46" s="29"/>
       <c r="V46" s="29"/>
       <c r="W46" s="29"/>
@@ -2720,15 +2748,15 @@
     </row>
     <row r="47" spans="1:31">
       <c r="B47" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="81">
-        <f>C44*0.03</f>
-        <v>1800</v>
-      </c>
-      <c r="D47" s="82"/>
+        <v>18</v>
+      </c>
+      <c r="C47" s="84">
+        <v>30000</v>
+      </c>
+      <c r="D47" s="85"/>
       <c r="E47" s="10">
-        <v>3</v>
+        <f>C47/C45*100</f>
+        <v>47.404168847909865</v>
       </c>
       <c r="M47" s="29"/>
       <c r="N47" s="29"/>
@@ -2752,15 +2780,16 @@
     </row>
     <row r="48" spans="1:31">
       <c r="B48" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="81">
-        <f>C44*0.02</f>
-        <v>1200</v>
-      </c>
-      <c r="D48" s="82"/>
+        <v>19</v>
+      </c>
+      <c r="C48" s="86">
+        <f>C45-C47</f>
+        <v>33285.573250426802</v>
+      </c>
+      <c r="D48" s="86"/>
       <c r="E48" s="10">
-        <v>2</v>
+        <f>100-E47</f>
+        <v>52.595831152090135</v>
       </c>
       <c r="M48" s="29"/>
       <c r="N48" s="29"/>
@@ -2782,16 +2811,80 @@
       <c r="AD48" s="29"/>
       <c r="AE48" s="29"/>
     </row>
+    <row r="49" spans="2:31">
+      <c r="B49" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="81">
+        <f>C46*0.03</f>
+        <v>1800</v>
+      </c>
+      <c r="D49" s="82"/>
+      <c r="E49" s="10">
+        <v>3</v>
+      </c>
+      <c r="M49" s="29"/>
+      <c r="N49" s="29"/>
+      <c r="O49" s="29"/>
+      <c r="P49" s="29"/>
+      <c r="Q49" s="29"/>
+      <c r="R49" s="29"/>
+      <c r="S49" s="29"/>
+      <c r="T49" s="29"/>
+      <c r="U49" s="29"/>
+      <c r="V49" s="29"/>
+      <c r="W49" s="29"/>
+      <c r="X49" s="29"/>
+      <c r="Y49" s="29"/>
+      <c r="Z49" s="29"/>
+      <c r="AA49" s="29"/>
+      <c r="AB49" s="29"/>
+      <c r="AC49" s="29"/>
+      <c r="AD49" s="29"/>
+      <c r="AE49" s="29"/>
+    </row>
+    <row r="50" spans="2:31">
+      <c r="B50" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="81">
+        <f>C46*0.02</f>
+        <v>1200</v>
+      </c>
+      <c r="D50" s="82"/>
+      <c r="E50" s="10">
+        <v>2</v>
+      </c>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="29"/>
+      <c r="Q50" s="29"/>
+      <c r="R50" s="29"/>
+      <c r="S50" s="29"/>
+      <c r="T50" s="29"/>
+      <c r="U50" s="29"/>
+      <c r="V50" s="29"/>
+      <c r="W50" s="29"/>
+      <c r="X50" s="29"/>
+      <c r="Y50" s="29"/>
+      <c r="Z50" s="29"/>
+      <c r="AA50" s="29"/>
+      <c r="AB50" s="29"/>
+      <c r="AC50" s="29"/>
+      <c r="AD50" s="29"/>
+      <c r="AE50" s="29"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="C48:D48"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -2811,10 +2904,1246 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1">
+      <c r="A1" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="22.5">
+      <c r="A2" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1">
+      <c r="A3" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1">
+      <c r="A4" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+    </row>
+    <row r="5" spans="1:13" ht="18.75">
+      <c r="A5" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+    </row>
+    <row r="6" spans="1:13" ht="18.75">
+      <c r="A6" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75">
+      <c r="A7" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="1" customFormat="1" ht="45">
+      <c r="A9" s="21">
+        <v>1</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="35"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="24"/>
+    </row>
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="30">
+      <c r="A10" s="38"/>
+      <c r="B10" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="40">
+        <v>3</v>
+      </c>
+      <c r="D10" s="10">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1.83</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" ref="F10:F16" si="0">PRODUCT(C10:E10)</f>
+        <v>13.889699999999999</v>
+      </c>
+      <c r="G10" s="36">
+        <f t="shared" ref="G10:G16" si="1">F10</f>
+        <v>13.889699999999999</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="11"/>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="11" spans="1:13" s="1" customFormat="1">
+      <c r="A11" s="38"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40">
+        <v>1</v>
+      </c>
+      <c r="D11" s="10">
+        <f>22/12/3.281</f>
+        <v>0.55877273189068366</v>
+      </c>
+      <c r="E11" s="10">
+        <v>1.83</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="0"/>
+        <v>1.0225540993599511</v>
+      </c>
+      <c r="G11" s="36">
+        <f t="shared" si="1"/>
+        <v>1.0225540993599511</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="11"/>
+      <c r="M11" s="12"/>
+    </row>
+    <row r="12" spans="1:13" s="1" customFormat="1">
+      <c r="A12" s="38"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="40">
+        <f>3</f>
+        <v>3</v>
+      </c>
+      <c r="D12" s="10">
+        <f>0.7-1.5/12/3.281</f>
+        <v>0.66190185918927158</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1.83</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="0"/>
+        <v>3.6338412069491013</v>
+      </c>
+      <c r="G12" s="36">
+        <f t="shared" si="1"/>
+        <v>3.6338412069491013</v>
+      </c>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="11"/>
+      <c r="M12" s="12"/>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1">
+      <c r="A13" s="38"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40">
+        <v>3</v>
+      </c>
+      <c r="D13" s="10">
+        <f>10/3.281</f>
+        <v>3.047851264858275</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1.83</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="0"/>
+        <v>16.73270344407193</v>
+      </c>
+      <c r="G13" s="36">
+        <f t="shared" si="1"/>
+        <v>16.73270344407193</v>
+      </c>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="11"/>
+      <c r="M13" s="12"/>
+    </row>
+    <row r="14" spans="1:13" s="1" customFormat="1">
+      <c r="A14" s="38"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="40">
+        <v>3</v>
+      </c>
+      <c r="D14" s="10">
+        <f>7.5/3.281</f>
+        <v>2.2858884486437061</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1.83</v>
+      </c>
+      <c r="F14" s="10">
+        <f t="shared" si="0"/>
+        <v>12.549527583053948</v>
+      </c>
+      <c r="G14" s="36">
+        <f t="shared" si="1"/>
+        <v>12.549527583053948</v>
+      </c>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="11"/>
+      <c r="M14" s="12"/>
+    </row>
+    <row r="15" spans="1:13" s="1" customFormat="1">
+      <c r="A15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="40">
+        <v>3</v>
+      </c>
+      <c r="D15" s="10">
+        <f>7/3.281</f>
+        <v>2.1334958854007922</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1.83</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" si="0"/>
+        <v>11.712892410850349</v>
+      </c>
+      <c r="G15" s="36">
+        <f t="shared" si="1"/>
+        <v>11.712892410850349</v>
+      </c>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="11"/>
+      <c r="M15" s="12"/>
+    </row>
+    <row r="16" spans="1:13" s="1" customFormat="1">
+      <c r="A16" s="38"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40">
+        <v>2</v>
+      </c>
+      <c r="D16" s="10">
+        <f>4.5</f>
+        <v>4.5</v>
+      </c>
+      <c r="E16" s="10">
+        <v>1.83</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="0"/>
+        <v>16.47</v>
+      </c>
+      <c r="G16" s="36">
+        <f t="shared" si="1"/>
+        <v>16.47</v>
+      </c>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="11"/>
+      <c r="M16" s="12"/>
+    </row>
+    <row r="17" spans="1:15" s="1" customFormat="1">
+      <c r="A17" s="21"/>
+      <c r="B17" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="27">
+        <f>SUM(G10:G16)</f>
+        <v>76.011218744285287</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="26">
+        <v>181.17</v>
+      </c>
+      <c r="J17" s="27">
+        <f>G17*I17</f>
+        <v>13770.952499902165</v>
+      </c>
+      <c r="K17" s="24"/>
+    </row>
+    <row r="18" spans="1:15" s="1" customFormat="1">
+      <c r="A18" s="21"/>
+      <c r="B18" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27">
+        <f>0.13*G17*(1871.42/18.94)</f>
+        <v>976.36530874952211</v>
+      </c>
+      <c r="K18" s="24"/>
+    </row>
+    <row r="19" spans="1:15" s="1" customFormat="1">
+      <c r="A19" s="21"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="1:15" s="1" customFormat="1">
+      <c r="A20" s="38">
+        <v>2</v>
+      </c>
+      <c r="B20" s="74" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="40"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="11"/>
+      <c r="M20" s="12"/>
+    </row>
+    <row r="21" spans="1:15" s="1" customFormat="1">
+      <c r="A21" s="38"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="40">
+        <v>1</v>
+      </c>
+      <c r="D21" s="10">
+        <v>4</v>
+      </c>
+      <c r="E21" s="10">
+        <f>7.5/3.281</f>
+        <v>2.2858884486437061</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="36">
+        <f>PRODUCT(C21:F21)</f>
+        <v>9.1435537945748244</v>
+      </c>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="11"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="1">
+        <f>D21*5</f>
+        <v>20</v>
+      </c>
+      <c r="O21" s="1">
+        <f>4.5</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="1" customFormat="1">
+      <c r="A22" s="21"/>
+      <c r="B22" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="27">
+        <f>SUM(G21:G21)</f>
+        <v>9.1435537945748244</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="26">
+        <f>Sheet1!H10/10</f>
+        <v>249.75</v>
+      </c>
+      <c r="J22" s="27">
+        <f>G22*I22</f>
+        <v>2283.6025601950623</v>
+      </c>
+      <c r="K22" s="24"/>
+    </row>
+    <row r="23" spans="1:15" s="1" customFormat="1" hidden="1">
+      <c r="A23" s="21"/>
+      <c r="B23" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="27">
+        <f>0*0.13*G22*5298.54/10</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="1:15" s="1" customFormat="1">
+      <c r="A24" s="21"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A25" s="21">
+        <v>3</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="24"/>
+    </row>
+    <row r="26" spans="1:15" s="1" customFormat="1">
+      <c r="A26" s="21"/>
+      <c r="B26" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="22">
+        <v>1</v>
+      </c>
+      <c r="D26" s="23">
+        <f>D37</f>
+        <v>4.5</v>
+      </c>
+      <c r="E26" s="24">
+        <f>10/3.281</f>
+        <v>3.047851264858275</v>
+      </c>
+      <c r="F26" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="G26" s="36">
+        <f t="shared" ref="G26" si="2">PRODUCT(C26:F26)</f>
+        <v>2.0572996037793354</v>
+      </c>
+      <c r="H26" s="25"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="24"/>
+    </row>
+    <row r="27" spans="1:15" s="1" customFormat="1">
+      <c r="A27" s="21"/>
+      <c r="B27" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="27">
+        <f>SUM(G26:G26)</f>
+        <v>2.0572996037793354</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="26">
+        <v>663.31</v>
+      </c>
+      <c r="J27" s="27">
+        <f>G27*I27</f>
+        <v>1364.6274001828708</v>
+      </c>
+      <c r="K27" s="24"/>
+    </row>
+    <row r="28" spans="1:15" s="1" customFormat="1">
+      <c r="A28" s="21"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="24"/>
+    </row>
+    <row r="29" spans="1:15" s="1" customFormat="1" ht="30">
+      <c r="A29" s="21">
+        <v>4</v>
+      </c>
+      <c r="B29" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="24"/>
+    </row>
+    <row r="30" spans="1:15" s="1" customFormat="1">
+      <c r="A30" s="21"/>
+      <c r="B30" s="39" t="str">
+        <f>B26</f>
+        <v>-for passage flooring</v>
+      </c>
+      <c r="C30" s="22">
+        <v>1</v>
+      </c>
+      <c r="D30" s="23">
+        <v>4</v>
+      </c>
+      <c r="E30" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="F30" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="G30" s="36">
+        <f t="shared" ref="G30" si="3">PRODUCT(C30:F30)</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="H30" s="25"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="24"/>
+    </row>
+    <row r="31" spans="1:15" s="1" customFormat="1">
+      <c r="A31" s="21"/>
+      <c r="B31" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="22"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="27">
+        <f>SUM(G30:G30)</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="26">
+        <v>4473.1499999999996</v>
+      </c>
+      <c r="J31" s="27">
+        <f>G31*I31</f>
+        <v>4025.8349999999991</v>
+      </c>
+      <c r="K31" s="24"/>
+    </row>
+    <row r="32" spans="1:15" s="1" customFormat="1">
+      <c r="A32" s="21"/>
+      <c r="B32" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="22"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="27">
+        <f>0.13*G31*3093.15</f>
+        <v>361.89855</v>
+      </c>
+      <c r="K32" s="24"/>
+      <c r="M32" s="1">
+        <f>4434</f>
+        <v>4434</v>
+      </c>
+      <c r="N32" s="1" t="e">
+        <f>(PRODUCT(#REF!))*0.15+(PRODUCT(#REF!))*0.15+(PRODUCT(C30:E30))*0.15</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O32" s="1" t="e">
+        <f>N32*M32</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" s="1" customFormat="1">
+      <c r="A33" s="21"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="24"/>
+    </row>
+    <row r="34" spans="1:31" s="1" customFormat="1" ht="30">
+      <c r="A34" s="21">
+        <v>5</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="24"/>
+    </row>
+    <row r="35" spans="1:31" s="1" customFormat="1">
+      <c r="A35" s="21"/>
+      <c r="B35" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="22">
+        <v>1</v>
+      </c>
+      <c r="D35" s="23">
+        <v>3</v>
+      </c>
+      <c r="E35" s="24">
+        <v>2.5</v>
+      </c>
+      <c r="F35" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="G35" s="36">
+        <f>PRODUCT(C35:F35)</f>
+        <v>0.375</v>
+      </c>
+      <c r="H35" s="25"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="24"/>
+    </row>
+    <row r="36" spans="1:31" s="1" customFormat="1">
+      <c r="A36" s="21"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="22">
+        <v>1</v>
+      </c>
+      <c r="D36" s="23">
+        <v>4.5</v>
+      </c>
+      <c r="E36" s="24">
+        <v>2.5</v>
+      </c>
+      <c r="F36" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="G36" s="36">
+        <f t="shared" ref="G36:G37" si="4">PRODUCT(C36:F36)</f>
+        <v>1.125</v>
+      </c>
+      <c r="H36" s="25"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="24"/>
+    </row>
+    <row r="37" spans="1:31" s="1" customFormat="1">
+      <c r="A37" s="21"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="22">
+        <v>1</v>
+      </c>
+      <c r="D37" s="23">
+        <v>4.5</v>
+      </c>
+      <c r="E37" s="24">
+        <f>(2.8+2.2)/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="F37" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="G37" s="36">
+        <f t="shared" si="4"/>
+        <v>1.125</v>
+      </c>
+      <c r="H37" s="25"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="24"/>
+    </row>
+    <row r="38" spans="1:31" s="1" customFormat="1">
+      <c r="A38" s="21"/>
+      <c r="B38" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="27">
+        <f>SUM(G35:G37)</f>
+        <v>2.625</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="I38" s="26">
+        <v>12983.1</v>
+      </c>
+      <c r="J38" s="27">
+        <f>G38*I38</f>
+        <v>34080.637500000004</v>
+      </c>
+      <c r="K38" s="24"/>
+    </row>
+    <row r="39" spans="1:31" s="1" customFormat="1">
+      <c r="A39" s="21"/>
+      <c r="B39" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="22"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="27">
+        <f>0.13*G38*8078.11</f>
+        <v>2756.6550374999997</v>
+      </c>
+      <c r="K39" s="24"/>
+    </row>
+    <row r="40" spans="1:31" s="1" customFormat="1">
+      <c r="A40" s="21"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="24"/>
+    </row>
+    <row r="41" spans="1:31" s="1" customFormat="1">
+      <c r="A41" s="21">
+        <v>6</v>
+      </c>
+      <c r="B41" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="22">
+        <v>1</v>
+      </c>
+      <c r="D41" s="23"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="36">
+        <f>PRODUCT(C41:F41)</f>
+        <v>1</v>
+      </c>
+      <c r="H41" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="I41" s="26">
+        <v>500</v>
+      </c>
+      <c r="J41" s="27">
+        <f>G41*I41</f>
+        <v>500</v>
+      </c>
+      <c r="K41" s="24"/>
+    </row>
+    <row r="42" spans="1:31" s="1" customFormat="1">
+      <c r="A42" s="21"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="24"/>
+    </row>
+    <row r="43" spans="1:31">
+      <c r="A43" s="9"/>
+      <c r="B43" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7">
+        <f>SUM(J10:J41)</f>
+        <v>60120.573856529627</v>
+      </c>
+      <c r="K43" s="4"/>
+      <c r="M43" s="29"/>
+      <c r="P43" s="32"/>
+      <c r="Q43" s="32"/>
+    </row>
+    <row r="44" spans="1:31">
+      <c r="M44" s="29"/>
+      <c r="N44" s="30"/>
+      <c r="O44" s="30"/>
+      <c r="P44" s="31"/>
+      <c r="R44" s="30"/>
+      <c r="S44" s="30"/>
+      <c r="T44" s="30"/>
+      <c r="U44" s="29"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
+      <c r="AA44" s="29"/>
+      <c r="AB44" s="29"/>
+      <c r="AC44" s="29"/>
+      <c r="AD44" s="29"/>
+      <c r="AE44" s="29"/>
+    </row>
+    <row r="45" spans="1:31" s="1" customFormat="1">
+      <c r="B45" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="86">
+        <f>J43</f>
+        <v>60120.573856529627</v>
+      </c>
+      <c r="D45" s="86"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="16"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="30"/>
+      <c r="O45" s="30"/>
+      <c r="P45" s="30"/>
+      <c r="Q45" s="30"/>
+      <c r="R45" s="30"/>
+      <c r="S45" s="30"/>
+      <c r="T45" s="30"/>
+      <c r="U45" s="12"/>
+      <c r="V45" s="12"/>
+      <c r="W45" s="12"/>
+      <c r="X45" s="12"/>
+      <c r="Y45" s="12"/>
+      <c r="Z45" s="12"/>
+      <c r="AA45" s="12"/>
+      <c r="AB45" s="12"/>
+      <c r="AC45" s="12"/>
+      <c r="AD45" s="12"/>
+      <c r="AE45" s="12"/>
+    </row>
+    <row r="46" spans="1:31" s="1" customFormat="1" hidden="1">
+      <c r="B46" s="96" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="97">
+        <f>J43</f>
+        <v>60120.573856529627</v>
+      </c>
+      <c r="D46" s="98"/>
+      <c r="E46" s="99">
+        <v>100</v>
+      </c>
+      <c r="F46" s="12"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="16"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="30"/>
+      <c r="O46" s="30"/>
+      <c r="P46" s="30"/>
+      <c r="Q46" s="30"/>
+      <c r="R46" s="30"/>
+      <c r="S46" s="30"/>
+      <c r="T46" s="30"/>
+      <c r="U46" s="12"/>
+      <c r="V46" s="12"/>
+      <c r="W46" s="12"/>
+      <c r="X46" s="12"/>
+      <c r="Y46" s="12"/>
+      <c r="Z46" s="12"/>
+      <c r="AA46" s="12"/>
+      <c r="AB46" s="12"/>
+      <c r="AC46" s="12"/>
+      <c r="AD46" s="12"/>
+      <c r="AE46" s="12"/>
+    </row>
+    <row r="47" spans="1:31" hidden="1">
+      <c r="B47" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="84">
+        <v>60000</v>
+      </c>
+      <c r="D47" s="85"/>
+      <c r="E47" s="10"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="30"/>
+      <c r="O47" s="30"/>
+      <c r="P47" s="30"/>
+      <c r="Q47" s="30"/>
+      <c r="R47" s="30"/>
+      <c r="S47" s="30"/>
+      <c r="T47" s="30"/>
+      <c r="U47" s="29"/>
+      <c r="V47" s="29"/>
+      <c r="W47" s="29"/>
+      <c r="X47" s="29"/>
+      <c r="Y47" s="29"/>
+      <c r="Z47" s="29"/>
+      <c r="AA47" s="29"/>
+      <c r="AB47" s="29"/>
+      <c r="AC47" s="29"/>
+      <c r="AD47" s="29"/>
+      <c r="AE47" s="29"/>
+    </row>
+    <row r="48" spans="1:31" hidden="1">
+      <c r="B48" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="84">
+        <v>30000</v>
+      </c>
+      <c r="D48" s="85"/>
+      <c r="E48" s="10">
+        <f>C48/C46*100</f>
+        <v>49.8997232987019</v>
+      </c>
+      <c r="M48" s="29"/>
+      <c r="N48" s="29"/>
+      <c r="O48" s="29"/>
+      <c r="P48" s="29"/>
+      <c r="Q48" s="29"/>
+      <c r="R48" s="29"/>
+      <c r="S48" s="29"/>
+      <c r="T48" s="29"/>
+      <c r="U48" s="29"/>
+      <c r="V48" s="29"/>
+      <c r="W48" s="29"/>
+      <c r="X48" s="29"/>
+      <c r="Y48" s="29"/>
+      <c r="Z48" s="29"/>
+      <c r="AA48" s="29"/>
+      <c r="AB48" s="29"/>
+      <c r="AC48" s="29"/>
+      <c r="AD48" s="29"/>
+      <c r="AE48" s="29"/>
+    </row>
+    <row r="49" spans="2:31" hidden="1">
+      <c r="B49" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="86">
+        <f>C46-C48</f>
+        <v>30120.573856529627</v>
+      </c>
+      <c r="D49" s="86"/>
+      <c r="E49" s="10">
+        <f>100-E48</f>
+        <v>50.1002767012981</v>
+      </c>
+      <c r="M49" s="29"/>
+      <c r="N49" s="29"/>
+      <c r="O49" s="29"/>
+      <c r="P49" s="29"/>
+      <c r="Q49" s="29"/>
+      <c r="R49" s="29"/>
+      <c r="S49" s="29"/>
+      <c r="T49" s="29"/>
+      <c r="U49" s="29"/>
+      <c r="V49" s="29"/>
+      <c r="W49" s="29"/>
+      <c r="X49" s="29"/>
+      <c r="Y49" s="29"/>
+      <c r="Z49" s="29"/>
+      <c r="AA49" s="29"/>
+      <c r="AB49" s="29"/>
+      <c r="AC49" s="29"/>
+      <c r="AD49" s="29"/>
+      <c r="AE49" s="29"/>
+    </row>
+    <row r="50" spans="2:31" hidden="1">
+      <c r="B50" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="81">
+        <f>C47*0.03</f>
+        <v>1800</v>
+      </c>
+      <c r="D50" s="82"/>
+      <c r="E50" s="10">
+        <v>3</v>
+      </c>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="29"/>
+      <c r="Q50" s="29"/>
+      <c r="R50" s="29"/>
+      <c r="S50" s="29"/>
+      <c r="T50" s="29"/>
+      <c r="U50" s="29"/>
+      <c r="V50" s="29"/>
+      <c r="W50" s="29"/>
+      <c r="X50" s="29"/>
+      <c r="Y50" s="29"/>
+      <c r="Z50" s="29"/>
+      <c r="AA50" s="29"/>
+      <c r="AB50" s="29"/>
+      <c r="AC50" s="29"/>
+      <c r="AD50" s="29"/>
+      <c r="AE50" s="29"/>
+    </row>
+    <row r="51" spans="2:31" hidden="1">
+      <c r="B51" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="81">
+        <f>C47*0.02</f>
+        <v>1200</v>
+      </c>
+      <c r="D51" s="82"/>
+      <c r="E51" s="10">
+        <v>2</v>
+      </c>
+      <c r="M51" s="29"/>
+      <c r="N51" s="29"/>
+      <c r="O51" s="29"/>
+      <c r="P51" s="29"/>
+      <c r="Q51" s="29"/>
+      <c r="R51" s="29"/>
+      <c r="S51" s="29"/>
+      <c r="T51" s="29"/>
+      <c r="U51" s="29"/>
+      <c r="V51" s="29"/>
+      <c r="W51" s="29"/>
+      <c r="X51" s="29"/>
+      <c r="Y51" s="29"/>
+      <c r="Z51" s="29"/>
+      <c r="AA51" s="29"/>
+      <c r="AB51" s="29"/>
+      <c r="AC51" s="29"/>
+      <c r="AD51" s="29"/>
+      <c r="AE51" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;LPrepared By:&amp;CChecked By:&amp;RApproved By: </oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2837,7 +4166,7 @@
         <v>#REF!</v>
       </c>
       <c r="B1" s="87" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C1" s="88"/>
       <c r="D1" s="88"/>
@@ -2933,7 +4262,7 @@
         <v>52</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="D6" s="56">
         <v>12</v>

</xml_diff>